<commit_message>
Calculo de volumenes para matrices. Super matrices. Regresa excel.
</commit_message>
<xml_diff>
--- a/VerificacionCompuestos/DatosPruebaMvsN.xlsx
+++ b/VerificacionCompuestos/DatosPruebaMvsN.xlsx
@@ -1,29 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://comunidadunammx-my.sharepoint.com/personal/pamema_comunidad_unam_mx/Documents/Programación/Matemáticas/Matlab/Proyecto Ana/VerificacionCompuestos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C633A1C-C859-41CB-97B6-F799DD8C782F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{07B066D3-0FBB-4851-948D-1C1B43A25F31}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" xr2:uid="{F0659778-C3FA-4246-A23C-D9F175EA623A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16389" windowHeight="10029" xr2:uid="{F0659778-C3FA-4246-A23C-D9F175EA623A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -48,8 +43,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -83,9 +86,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,15 +404,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E623AF-0393-4572-BA98-9F6CD50E2EA0}">
-  <dimension ref="B1:C402"/>
+  <dimension ref="B1:C403"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A375" workbookViewId="0">
+      <selection activeCell="C404" sqref="C404"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -416,7 +420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -424,7 +428,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B3">
         <v>0.5535201807412834</v>
       </c>
@@ -432,7 +436,7 @@
         <v>0.79824204677291311</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B4">
         <v>0.56169792694965448</v>
       </c>
@@ -440,7 +444,7 @@
         <v>0.82327307502467917</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B5">
         <v>0.56733808490858373</v>
       </c>
@@ -448,7 +452,7 @@
         <v>0.83639231484350773</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B6">
         <v>0.56739773287333661</v>
       </c>
@@ -456,7 +460,7 @@
         <v>0.83336619024149816</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B7">
         <v>0.56311151625645695</v>
       </c>
@@ -464,7 +468,7 @@
         <v>0.81622910969310225</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B8">
         <v>0.55514309663513361</v>
       </c>
@@ -472,7 +476,7 @@
         <v>0.79375943000838234</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B9">
         <v>0.54544382188145091</v>
       </c>
@@ -480,7 +484,7 @@
         <v>0.77130875847832503</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B10">
         <v>0.54110753003222967</v>
       </c>
@@ -488,7 +492,7 @@
         <v>0.75941634925285673</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B11">
         <v>0.54243260703588414</v>
       </c>
@@ -496,7 +500,7 @@
         <v>0.75809420332413224</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B12">
         <v>0.54660515732197779</v>
       </c>
@@ -504,7 +508,7 @@
         <v>0.75999704281996705</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B13">
         <v>0.5477377983612397</v>
       </c>
@@ -512,7 +516,7 @@
         <v>0.75729485809286301</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B14">
         <v>0.54664445502141834</v>
       </c>
@@ -520,7 +524,7 @@
         <v>0.75160102332222756</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B15">
         <v>0.54247939764036279</v>
       </c>
@@ -528,7 +532,7 @@
         <v>0.74256358569988734</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B16">
         <v>0.53625235404896432</v>
       </c>
@@ -536,7 +540,7 @@
         <v>0.73294197269303207</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B17">
         <v>0.53064921404779997</v>
       </c>
@@ -544,7 +548,7 @@
         <v>0.72644363933851452</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B18">
         <v>0.52886970722034299</v>
       </c>
@@ -552,7 +556,7 @@
         <v>0.72706812084451189</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B19">
         <v>0.5301958491669102</v>
       </c>
@@ -560,7 +564,7 @@
         <v>0.73385676702718505</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B20">
         <v>0.53471977440958762</v>
       </c>
@@ -568,7 +572,7 @@
         <v>0.74119551169075326</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B21">
         <v>0.54161490683229807</v>
       </c>
@@ -576,7 +580,7 @@
         <v>0.74463531499556346</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B22">
         <v>0.54857721157280626</v>
       </c>
@@ -584,7 +588,7 @@
         <v>0.74164602928920109</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B23">
         <v>0.55403466826060965</v>
       </c>
@@ -592,7 +596,7 @@
         <v>0.73523789599521816</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B24">
         <v>0.55881294964028771</v>
       </c>
@@ -600,7 +604,7 @@
         <v>0.73139688249400481</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B25">
         <v>0.55683847161052247</v>
       </c>
@@ -608,7 +612,7 @@
         <v>0.7243149625044637</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B26">
         <v>0.55120145702367662</v>
       </c>
@@ -616,7 +620,7 @@
         <v>0.71596028435462078</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B27">
         <v>0.54431778527393282</v>
       </c>
@@ -624,7 +628,7 @@
         <v>0.71053158078399448</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B28">
         <v>0.53700596030322323</v>
       </c>
@@ -632,7 +636,7 @@
         <v>0.70855216711995839</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B29">
         <v>0.52996298010180465</v>
       </c>
@@ -640,7 +644,7 @@
         <v>0.7101457658491438</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B30">
         <v>0.52833499035031284</v>
       </c>
@@ -648,7 +652,7 @@
         <v>0.72116439557868872</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B31">
         <v>0.53039694838478968</v>
       </c>
@@ -656,7 +660,7 @@
         <v>0.74005662176659914</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B32">
         <v>0.53475288851249181</v>
       </c>
@@ -664,7 +668,7 @@
         <v>0.75629363014941631</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B33">
         <v>0.54058015267175563</v>
       </c>
@@ -672,7 +676,7 @@
         <v>0.7664030534351145</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B34">
         <v>0.54587831207065751</v>
       </c>
@@ -680,7 +684,7 @@
         <v>0.76909102060843981</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B35">
         <v>0.54735939223134411</v>
       </c>
@@ -688,7 +692,7 @@
         <v>0.76468570028182814</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B36">
         <v>0.54590343818580833</v>
       </c>
@@ -696,7 +700,7 @@
         <v>0.75714459887832231</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B37">
         <v>0.54147941212194828</v>
       </c>
@@ -704,7 +708,7 @@
         <v>0.75207032673387586</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B38">
         <v>0.53520358700920989</v>
       </c>
@@ -712,7 +716,7 @@
         <v>0.75078829374697054</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B39">
         <v>0.5315901489814534</v>
       </c>
@@ -720,7 +724,7 @@
         <v>0.75799331103678935</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B40">
         <v>0.53514613392526822</v>
       </c>
@@ -728,7 +732,7 @@
         <v>0.77457084720680724</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B41">
         <v>0.54480670997036007</v>
       </c>
@@ -736,7 +740,7 @@
         <v>0.79284543103991922</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B42">
         <v>0.55123199999999994</v>
       </c>
@@ -744,7 +748,7 @@
         <v>0.79430015999999992</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B43">
         <v>0.55533303184960281</v>
       </c>
@@ -752,7 +756,7 @@
         <v>0.78181536274953178</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B44">
         <v>0.55765226444560123</v>
       </c>
@@ -760,7 +764,7 @@
         <v>0.76880921395106716</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B45">
         <v>0.55883123689727454</v>
       </c>
@@ -768,7 +772,7 @@
         <v>0.76096698113207539</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B46">
         <v>0.55881577212185152</v>
       </c>
@@ -776,7 +780,7 @@
         <v>0.75939074245021754</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B47">
         <v>0.5574107202014178</v>
       </c>
@@ -784,7 +788,7 @@
         <v>0.76235208374743257</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B48">
         <v>0.55483184899641103</v>
       </c>
@@ -792,7 +796,7 @@
         <v>0.76840821480792243</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B49">
         <v>0.55442448436460412</v>
       </c>
@@ -800,7 +804,7 @@
         <v>0.77668928809048565</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B50">
         <v>0.55667087681978322</v>
       </c>
@@ -808,7 +812,7 @@
         <v>0.78653460081100834</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B51">
         <v>0.56088340628730604</v>
       </c>
@@ -816,7 +820,7 @@
         <v>0.79514060220188354</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B52">
         <v>0.56504494976203068</v>
       </c>
@@ -824,7 +828,7 @@
         <v>0.79988696456901109</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B53">
         <v>0.56937767533750416</v>
       </c>
@@ -832,7 +836,7 @@
         <v>0.80036088244978598</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B54">
         <v>0.57145666710371057</v>
       </c>
@@ -840,7 +844,7 @@
         <v>0.79708732135833227</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B55">
         <v>0.5715310380803339</v>
       </c>
@@ -848,7 +852,7 @@
         <v>0.78979786124152329</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B56">
         <v>0.57036461369082325</v>
       </c>
@@ -856,7 +860,7 @@
         <v>0.77716080564730283</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B57">
         <v>0.56901751909131748</v>
       </c>
@@ -864,7 +868,7 @@
         <v>0.75791631906564849</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B58">
         <v>0.56737543636940657</v>
       </c>
@@ -872,7 +876,7 @@
         <v>0.73560583941605839</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B59">
         <v>0.56312926020886744</v>
       </c>
@@ -880,7 +884,7 @@
         <v>0.71707272840973046</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B60">
         <v>0.55746172292934881</v>
       </c>
@@ -888,7 +892,7 @@
         <v>0.70838590665928791</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B61">
         <v>0.55149199417758366</v>
       </c>
@@ -896,7 +900,7 @@
         <v>0.70927583697234353</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B62">
         <v>0.54585415788522917</v>
       </c>
@@ -904,7 +908,7 @@
         <v>0.71301017643162523</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B63">
         <v>0.54065749143578334</v>
       </c>
@@ -912,7 +916,7 @@
         <v>0.71023919706713146</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B64">
         <v>0.53372065165309057</v>
       </c>
@@ -920,7 +924,7 @@
         <v>0.69881827982750366</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B65">
         <v>0.52594536562089944</v>
       </c>
@@ -928,7 +932,7 @@
         <v>0.68446856733866157</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B66">
         <v>0.51442650201852291</v>
       </c>
@@ -936,7 +940,7 @@
         <v>0.6698883875563999</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B67">
         <v>0.49861184948904247</v>
       </c>
@@ -944,7 +948,7 @@
         <v>0.65504046311063857</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B68">
         <v>0.48049655821615578</v>
       </c>
@@ -952,7 +956,7 @@
         <v>0.64147437783138206</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B69">
         <v>0.46610169491525427</v>
       </c>
@@ -960,7 +964,7 @@
         <v>0.63933684959108694</v>
       </c>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B70">
         <v>0.45356176735798015</v>
       </c>
@@ -968,7 +972,7 @@
         <v>0.65007754733994594</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B71">
         <v>0.45166676974457298</v>
       </c>
@@ -976,7 +980,7 @@
         <v>0.68136557610241844</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B72">
         <v>0.46036251048184224</v>
       </c>
@@ -984,7 +988,7 @@
         <v>0.72933754757143776</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B73">
         <v>0.47880839539607317</v>
       </c>
@@ -992,7 +996,7 @@
         <v>0.78719634394041993</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B74">
         <v>0.50732394366197175</v>
       </c>
@@ -1000,7 +1004,7 @@
         <v>0.84151760563380296</v>
       </c>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B75">
         <v>0.54566591586136737</v>
       </c>
@@ -1008,7 +1012,7 @@
         <v>0.88895589624355142</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B76">
         <v>0.56731461483081369</v>
       </c>
@@ -1016,7 +1020,7 @@
         <v>0.89884233261339108</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B77">
         <v>0.57519057519057515</v>
       </c>
@@ -1024,7 +1028,7 @@
         <v>0.87985169785169792</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B78">
         <v>0.57558293587705356</v>
       </c>
@@ -1032,7 +1036,7 @@
         <v>0.85216878643349236</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B79">
         <v>0.57404560594414555</v>
       </c>
@@ -1040,7 +1044,7 @@
         <v>0.82908147578785552</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B80">
         <v>0.5711252653927813</v>
       </c>
@@ -1048,7 +1052,7 @@
         <v>0.80882228050455851</v>
       </c>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B81">
         <v>0.56624374771257768</v>
       </c>
@@ -1056,7 +1060,7 @@
         <v>0.78672502134927413</v>
       </c>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B82">
         <v>0.56007393715341969</v>
       </c>
@@ -1064,7 +1068,7 @@
         <v>0.76305229264802332</v>
       </c>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B83">
         <v>0.5545731350275207</v>
       </c>
@@ -1072,7 +1076,7 @@
         <v>0.74100245930436814</v>
       </c>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B84">
         <v>0.55059299971073183</v>
       </c>
@@ -1080,7 +1084,7 @@
         <v>0.72293549320219852</v>
       </c>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B85">
         <v>0.54746871771323613</v>
       </c>
@@ -1088,7 +1092,7 @@
         <v>0.70832912409597071</v>
       </c>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B86">
         <v>0.54403019213174741</v>
       </c>
@@ -1096,7 +1100,7 @@
         <v>0.69743938700823427</v>
       </c>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B87">
         <v>0.54023972602739734</v>
       </c>
@@ -1104,7 +1108,7 @@
         <v>0.68807648401826504</v>
       </c>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B88">
         <v>0.53767319363334487</v>
       </c>
@@ -1112,7 +1116,7 @@
         <v>0.68230447727012489</v>
       </c>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B89">
         <v>0.53634894991922455</v>
       </c>
@@ -1120,7 +1124,7 @@
         <v>0.68156300484652665</v>
       </c>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B90">
         <v>0.53647292250233425</v>
       </c>
@@ -1128,7 +1132,7 @@
         <v>0.68823587768440708</v>
       </c>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B91">
         <v>0.54066559886100718</v>
       </c>
@@ -1136,7 +1140,7 @@
         <v>0.7057934389274485</v>
       </c>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B92">
         <v>0.54834413029000417</v>
       </c>
@@ -1144,7 +1148,7 @@
         <v>0.72795362353938364</v>
       </c>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B93">
         <v>0.5548189073050952</v>
       </c>
@@ -1152,7 +1156,7 @@
         <v>0.74392203806015955</v>
       </c>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B94">
         <v>0.55996783571472764</v>
       </c>
@@ -1160,7 +1164,7 @@
         <v>0.75664439908455505</v>
       </c>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B95">
         <v>0.56191538127981167</v>
       </c>
@@ -1168,7 +1172,7 @@
         <v>0.76922133432447493</v>
       </c>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B96">
         <v>0.55739017928655044</v>
       </c>
@@ -1176,7 +1180,7 @@
         <v>0.77809438728359315</v>
       </c>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B97">
         <v>0.54713763702801466</v>
       </c>
@@ -1184,7 +1188,7 @@
         <v>0.77728197320341053</v>
       </c>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B98">
         <v>0.54262574595055413</v>
       </c>
@@ -1192,7 +1196,7 @@
         <v>0.77762574595055423</v>
       </c>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B99">
         <v>0.54190698245183455</v>
       </c>
@@ -1200,7 +1204,7 @@
         <v>0.77590808688182611</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B100">
         <v>0.54338663691583</v>
       </c>
@@ -1208,7 +1212,7 @@
         <v>0.7713778356266271</v>
       </c>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B101">
         <v>0.54578411150696926</v>
       </c>
@@ -1216,7 +1220,7 @@
         <v>0.76493280830051891</v>
       </c>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B102">
         <v>0.54910601863510444</v>
       </c>
@@ -1224,7 +1228,7 @@
         <v>0.76273860488541934</v>
       </c>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B103">
         <v>0.55028952668680764</v>
       </c>
@@ -1232,7 +1236,7 @@
         <v>0.76506231117824774</v>
       </c>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B104">
         <v>0.55008457056944193</v>
       </c>
@@ -1240,7 +1244,7 @@
         <v>0.76898264737204802</v>
       </c>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B105">
         <v>0.54874027993779162</v>
       </c>
@@ -1248,7 +1252,7 @@
         <v>0.77204727838258169</v>
       </c>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B106">
         <v>0.54643628509719222</v>
       </c>
@@ -1256,7 +1260,7 @@
         <v>0.77209564949089793</v>
       </c>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B107">
         <v>0.5432468803523367</v>
       </c>
@@ -1264,7 +1268,7 @@
         <v>0.76596158551504789</v>
       </c>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B108">
         <v>0.53978586202701051</v>
       </c>
@@ -1272,7 +1276,7 @@
         <v>0.75758547268524146</v>
       </c>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B109">
         <v>0.53593939393939394</v>
       </c>
@@ -1280,7 +1284,7 @@
         <v>0.74886424242424254</v>
       </c>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B110">
         <v>0.53271934076587502</v>
       </c>
@@ -1288,7 +1292,7 @@
         <v>0.74401539020843432</v>
       </c>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B111">
         <v>0.53001579778830965</v>
       </c>
@@ -1296,7 +1300,7 @@
         <v>0.74454611738971932</v>
       </c>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B112">
         <v>0.52912027407316775</v>
       </c>
@@ -1304,7 +1308,7 @@
         <v>0.74907500305885233</v>
       </c>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B113">
         <v>0.5339962709757613</v>
       </c>
@@ -1312,7 +1316,7 @@
         <v>0.75986389061528903</v>
       </c>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B114">
         <v>0.54320203303684889</v>
       </c>
@@ -1320,7 +1324,7 @@
         <v>0.77566010165184252</v>
       </c>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B115">
         <v>0.55115106052767715</v>
       </c>
@@ -1328,7 +1332,7 @@
         <v>0.79123706673564398</v>
       </c>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B116">
         <v>0.55765322844968856</v>
       </c>
@@ -1336,7 +1340,7 @@
         <v>0.80695640773516886</v>
       </c>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B117">
         <v>0.56102868447082088</v>
       </c>
@@ -1344,7 +1348,7 @@
         <v>0.81763138806462243</v>
       </c>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B118">
         <v>0.55934980664612954</v>
       </c>
@@ -1352,7 +1356,7 @@
         <v>0.81813724847610925</v>
       </c>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B119">
         <v>0.55372700871248781</v>
       </c>
@@ -1360,7 +1364,7 @@
         <v>0.81016521458535007</v>
       </c>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B120">
         <v>0.54976394028327158</v>
       </c>
@@ -1368,7 +1372,7 @@
         <v>0.80390519331376797</v>
       </c>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B121">
         <v>0.54651162790697683</v>
       </c>
@@ -1376,7 +1380,7 @@
         <v>0.79853513650151675</v>
       </c>
     </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B122">
         <v>0.54398496240601502</v>
       </c>
@@ -1384,7 +1388,7 @@
         <v>0.79471491228070179</v>
       </c>
     </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B123">
         <v>0.54229072152134727</v>
       </c>
@@ -1392,7 +1396,7 @@
         <v>0.7930557454477658</v>
       </c>
     </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B124">
         <v>0.540960364914011</v>
       </c>
@@ -1400,7 +1404,7 @@
         <v>0.79322628367133075</v>
       </c>
     </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B125">
         <v>0.53434275596800773</v>
       </c>
@@ -1408,7 +1412,7 @@
         <v>0.79308993223029478</v>
       </c>
     </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B126">
         <v>0.52488824453304328</v>
       </c>
@@ -1416,7 +1420,7 @@
         <v>0.79217953364745686</v>
       </c>
     </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B127">
         <v>0.51801503759398493</v>
       </c>
@@ -1424,7 +1428,7 @@
         <v>0.79593383458646616</v>
       </c>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B128">
         <v>0.51490645745322872</v>
       </c>
@@ -1432,7 +1436,7 @@
         <v>0.80373928786964388</v>
       </c>
     </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B129">
         <v>0.51525114155251139</v>
       </c>
@@ -1440,7 +1444,7 @@
         <v>0.81206149162861496</v>
       </c>
     </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B130">
         <v>0.52138066818433515</v>
       </c>
@@ -1448,7 +1452,7 @@
         <v>0.81747062080846589</v>
       </c>
     </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B131">
         <v>0.53207124174866116</v>
       </c>
@@ -1456,7 +1460,7 @@
         <v>0.8215904844937103</v>
       </c>
     </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B132">
         <v>0.54243658001879114</v>
       </c>
@@ -1464,7 +1468,7 @@
         <v>0.82087253366739765</v>
       </c>
     </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B133">
         <v>0.55199198195940868</v>
       </c>
@@ -1472,7 +1476,7 @@
         <v>0.81602981708844913</v>
       </c>
     </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B134">
         <v>0.5593241473907351</v>
       </c>
@@ -1480,7 +1484,7 @@
         <v>0.80746430575472294</v>
       </c>
     </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B135">
         <v>0.56151945645460155</v>
       </c>
@@ -1488,7 +1492,7 @@
         <v>0.797696726374305</v>
       </c>
     </row>
-    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B136">
         <v>0.55940775042651725</v>
       </c>
@@ -1496,7 +1500,7 @@
         <v>0.78889105532537174</v>
       </c>
     </row>
-    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B137">
         <v>0.55667430362956716</v>
       </c>
@@ -1504,7 +1508,7 @@
         <v>0.7878415531170867</v>
       </c>
     </row>
-    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B138">
         <v>0.55343693962940821</v>
       </c>
@@ -1512,7 +1516,7 @@
         <v>0.79293962940824858</v>
       </c>
     </row>
-    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B139">
         <v>0.55060848916592464</v>
       </c>
@@ -1520,7 +1524,7 @@
         <v>0.79887800534283171</v>
       </c>
     </row>
-    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B140">
         <v>0.54892812850646677</v>
       </c>
@@ -1528,7 +1532,7 @@
         <v>0.80414988484025285</v>
       </c>
     </row>
-    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B141">
         <v>0.54792426202516753</v>
       </c>
@@ -1536,7 +1540,7 @@
         <v>0.80639127366811725</v>
       </c>
     </row>
-    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B142">
         <v>0.54624649204864362</v>
       </c>
@@ -1544,7 +1548,7 @@
         <v>0.80250818521983169</v>
       </c>
     </row>
-    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B143">
         <v>0.54426629487626343</v>
       </c>
@@ -1552,7 +1556,7 @@
         <v>0.79106599279656098</v>
       </c>
     </row>
-    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B144">
         <v>0.54204204204204209</v>
       </c>
@@ -1560,7 +1564,7 @@
         <v>0.77665049665049679</v>
       </c>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B145">
         <v>0.53985861256394052</v>
       </c>
@@ -1568,7 +1572,7 @@
         <v>0.76270647738375774</v>
       </c>
     </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B146">
         <v>0.53808705612829322</v>
       </c>
@@ -1576,7 +1580,7 @@
         <v>0.75044730813287519</v>
       </c>
     </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B147">
         <v>0.54020618556701028</v>
       </c>
@@ -1584,7 +1588,7 @@
         <v>0.74239805269186721</v>
       </c>
     </row>
-    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B148">
         <v>0.54495349638305202</v>
       </c>
@@ -1592,7 +1596,7 @@
         <v>0.7401044896084511</v>
       </c>
     </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B149">
         <v>0.54781710745224022</v>
       </c>
@@ -1600,7 +1604,7 @@
         <v>0.74124490849635705</v>
       </c>
     </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B150">
         <v>0.54814941740918444</v>
       </c>
@@ -1608,7 +1612,7 @@
         <v>0.74401245145076533</v>
       </c>
     </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B151">
         <v>0.54697700823162088</v>
       </c>
@@ -1616,7 +1620,7 @@
         <v>0.74621061595231342</v>
       </c>
     </row>
-    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B152">
         <v>0.54596336499321574</v>
       </c>
@@ -1624,7 +1628,7 @@
         <v>0.74868781094527348</v>
       </c>
     </row>
-    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B153">
         <v>0.54500846023688665</v>
       </c>
@@ -1632,7 +1636,7 @@
         <v>0.75231754089114489</v>
       </c>
     </row>
-    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B154">
         <v>0.54450586642599275</v>
       </c>
@@ -1640,7 +1644,7 @@
         <v>0.75844652527075807</v>
       </c>
     </row>
-    <row r="155" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B155">
         <v>0.54439608884869728</v>
       </c>
@@ -1648,7 +1652,7 @@
         <v>0.76494658904651558</v>
       </c>
     </row>
-    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B156">
         <v>0.54428086070215176</v>
       </c>
@@ -1656,7 +1660,7 @@
         <v>0.7680628539071348</v>
       </c>
     </row>
-    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B157">
         <v>0.5439569770733087</v>
       </c>
@@ -1664,7 +1668,7 @@
         <v>0.7664489102745542</v>
       </c>
     </row>
-    <row r="158" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B158">
         <v>0.54296037032855371</v>
       </c>
@@ -1672,7 +1676,7 @@
         <v>0.76219769673704418</v>
       </c>
     </row>
-    <row r="159" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B159">
         <v>0.54308108717717374</v>
       </c>
@@ -1680,7 +1684,7 @@
         <v>0.75976091124393808</v>
       </c>
     </row>
-    <row r="160" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B160">
         <v>0.54400902170848608</v>
       </c>
@@ -1688,7 +1692,7 @@
         <v>0.75717507753030733</v>
       </c>
     </row>
-    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B161">
         <v>0.54450202794051383</v>
       </c>
@@ -1696,7 +1700,7 @@
         <v>0.75175135196034248</v>
       </c>
     </row>
-    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B162">
         <v>0.54380053908355797</v>
       </c>
@@ -1704,7 +1708,7 @@
         <v>0.74311938454627124</v>
       </c>
     </row>
-    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B163">
         <v>0.54242593627724989</v>
       </c>
@@ -1712,7 +1716,7 @@
         <v>0.73383566238121845</v>
       </c>
     </row>
-    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B164">
         <v>0.53966312746678524</v>
       </c>
@@ -1720,7 +1724,7 @@
         <v>0.72653010172883425</v>
       </c>
     </row>
-    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B165">
         <v>0.53618784530386743</v>
       </c>
@@ -1728,7 +1732,7 @@
         <v>0.72212707182320435</v>
       </c>
     </row>
-    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B166">
         <v>0.53418850473464008</v>
       </c>
@@ -1736,7 +1740,7 @@
         <v>0.72283252587535796</v>
       </c>
     </row>
-    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B167">
         <v>0.53404149925697619</v>
       </c>
@@ -1744,7 +1748,7 @@
         <v>0.72924376685563319</v>
       </c>
     </row>
-    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B168">
         <v>0.53509013727327859</v>
       </c>
@@ -1752,7 +1756,7 @@
         <v>0.73975136446331125</v>
       </c>
     </row>
-    <row r="169" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B169">
         <v>0.5358777783906018</v>
       </c>
@@ -1760,7 +1764,7 @@
         <v>0.74873476366444225</v>
       </c>
     </row>
-    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B170">
         <v>0.5362358776522459</v>
       </c>
@@ -1768,7 +1772,7 @@
         <v>0.75270377514466802</v>
       </c>
     </row>
-    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B171">
         <v>0.53558669964275896</v>
       </c>
@@ -1776,7 +1780,7 @@
         <v>0.74918219291013999</v>
       </c>
     </row>
-    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B172">
         <v>0.53391684901531733</v>
       </c>
@@ -1784,7 +1788,7 @@
         <v>0.74091794310722114</v>
       </c>
     </row>
-    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B173">
         <v>0.53128227428385066</v>
       </c>
@@ -1792,7 +1796,7 @@
         <v>0.72996249388487255</v>
       </c>
     </row>
-    <row r="174" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B174">
         <v>0.527419789700728</v>
       </c>
@@ -1800,7 +1804,7 @@
         <v>0.71641520625505517</v>
       </c>
     </row>
-    <row r="175" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B175">
         <v>0.52270541724543229</v>
       </c>
@@ -1808,7 +1812,7 @@
         <v>0.70135911956405594</v>
       </c>
     </row>
-    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B176">
         <v>0.5299020403745196</v>
       </c>
@@ -1816,7 +1820,7 @@
         <v>0.70630134762136709</v>
       </c>
     </row>
-    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B177">
         <v>0.5462803009194761</v>
       </c>
@@ -1824,7 +1828,7 @@
         <v>0.72987183059348004</v>
       </c>
     </row>
-    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B178">
         <v>0.56164148351648358</v>
       </c>
@@ -1832,7 +1836,7 @@
         <v>0.75581444597069602</v>
       </c>
     </row>
-    <row r="179" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B179">
         <v>0.5654402026832499</v>
       </c>
@@ -1840,7 +1844,7 @@
         <v>0.76329648183336218</v>
       </c>
     </row>
-    <row r="180" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B180">
         <v>0.56006613832031471</v>
       </c>
@@ -1848,7 +1852,7 @@
         <v>0.75372655225497465</v>
       </c>
     </row>
-    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B181">
         <v>0.55475113122171948</v>
       </c>
@@ -1856,7 +1860,7 @@
         <v>0.7422087104072399</v>
       </c>
     </row>
-    <row r="182" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B182">
         <v>0.54943264801707681</v>
       </c>
@@ -1864,7 +1868,7 @@
         <v>0.73065947646331875</v>
       </c>
     </row>
-    <row r="183" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B183">
         <v>0.54621330943311663</v>
       </c>
@@ -1872,7 +1876,7 @@
         <v>0.72294924938382255</v>
       </c>
     </row>
-    <row r="184" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B184">
         <v>0.54571989896154927</v>
       </c>
@@ -1880,7 +1884,7 @@
         <v>0.72112096547852944</v>
       </c>
     </row>
-    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B185">
         <v>0.54711657826430415</v>
       </c>
@@ -1888,7 +1892,7 @@
         <v>0.72446958582552756</v>
       </c>
     </row>
-    <row r="186" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B186">
         <v>0.55039508839747597</v>
       </c>
@@ -1896,7 +1900,7 @@
         <v>0.73141038030811201</v>
       </c>
     </row>
-    <row r="187" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B187">
         <v>0.55484832845920062</v>
       </c>
@@ -1904,7 +1908,7 @@
         <v>0.74069556740638787</v>
       </c>
     </row>
-    <row r="188" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B188">
         <v>0.55630928427709114</v>
       </c>
@@ -1912,7 +1916,7 @@
         <v>0.74622880137970682</v>
       </c>
     </row>
-    <row r="189" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B189">
         <v>0.55428375207462943</v>
       </c>
@@ -1920,7 +1924,7 @@
         <v>0.74811079951925818</v>
       </c>
     </row>
-    <row r="190" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B190">
         <v>0.5502894766715859</v>
       </c>
@@ -1928,7 +1932,7 @@
         <v>0.74821092064933581</v>
       </c>
     </row>
-    <row r="191" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B191">
         <v>0.54707608941070218</v>
       </c>
@@ -1936,7 +1940,7 @@
         <v>0.75218898171144732</v>
       </c>
     </row>
-    <row r="192" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B192">
         <v>0.54409532909898262</v>
       </c>
@@ -1944,7 +1948,7 @@
         <v>0.75903827778090049</v>
       </c>
     </row>
-    <row r="193" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B193">
         <v>0.54122586062132649</v>
       </c>
@@ -1952,7 +1956,7 @@
         <v>0.76620095158130408</v>
       </c>
     </row>
-    <row r="194" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B194">
         <v>0.53869744619159132</v>
       </c>
@@ -1960,7 +1964,7 @@
         <v>0.77181052748968426</v>
       </c>
     </row>
-    <row r="195" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B195">
         <v>0.53722960573875334</v>
       </c>
@@ -1968,7 +1972,7 @@
         <v>0.77547350275259974</v>
       </c>
     </row>
-    <row r="196" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B196">
         <v>0.53816645354978587</v>
       </c>
@@ -1976,7 +1980,7 @@
         <v>0.77930394173569795</v>
       </c>
     </row>
-    <row r="197" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B197">
         <v>0.5411050462292526</v>
       </c>
@@ -1984,7 +1988,7 @@
         <v>0.78192102038542943</v>
       </c>
     </row>
-    <row r="198" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B198">
         <v>0.54296395491574601</v>
       </c>
@@ -1992,7 +1996,7 @@
         <v>0.78007421046758185</v>
       </c>
     </row>
-    <row r="199" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B199">
         <v>0.54386945344808313</v>
       </c>
@@ -2000,7 +2004,7 @@
         <v>0.77293785626466971</v>
       </c>
     </row>
-    <row r="200" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B200">
         <v>0.54481251050950052</v>
       </c>
@@ -2008,7 +2012,7 @@
         <v>0.76581189395213278</v>
       </c>
     </row>
-    <row r="201" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B201">
         <v>0.54641266978526737</v>
       </c>
@@ -2016,7 +2020,7 @@
         <v>0.76321817054613084</v>
       </c>
     </row>
-    <row r="202" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B202">
         <v>0.5484951731970471</v>
       </c>
@@ -2024,7 +2028,7 @@
         <v>0.76499943214082911</v>
       </c>
     </row>
-    <row r="203" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B203">
         <v>0.54555750608754749</v>
       </c>
@@ -2032,7 +2036,7 @@
         <v>0.75705249447873624</v>
       </c>
     </row>
-    <row r="204" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B204">
         <v>0.53968343062415802</v>
       </c>
@@ -2040,7 +2044,7 @@
         <v>0.74019196228109563</v>
       </c>
     </row>
-    <row r="205" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B205">
         <v>0.53391526743022355</v>
       </c>
@@ -2048,7 +2052,7 @@
         <v>0.72146280440342492</v>
       </c>
     </row>
-    <row r="206" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B206">
         <v>0.52917172162788129</v>
       </c>
@@ -2056,7 +2060,7 @@
         <v>0.70716885408624675</v>
       </c>
     </row>
-    <row r="207" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B207">
         <v>0.52613393297866506</v>
       </c>
@@ -2064,7 +2068,7 @@
         <v>0.7006767948225745</v>
       </c>
     </row>
-    <row r="208" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B208">
         <v>0.5306867190091783</v>
       </c>
@@ -2072,7 +2076,7 @@
         <v>0.70580670131593493</v>
       </c>
     </row>
-    <row r="209" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B209">
         <v>0.54054814564691323</v>
       </c>
@@ -2080,7 +2084,7 @@
         <v>0.7170808711801453</v>
       </c>
     </row>
-    <row r="210" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B210">
         <v>0.54719235364396657</v>
       </c>
@@ -2088,7 +2092,7 @@
         <v>0.72196620583717364</v>
       </c>
     </row>
-    <row r="211" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B211">
         <v>0.55013132351261851</v>
       </c>
@@ -2096,7 +2100,7 @@
         <v>0.72191618134064184</v>
       </c>
     </row>
-    <row r="212" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B212">
         <v>0.55048488305761545</v>
       </c>
@@ -2104,7 +2108,7 @@
         <v>0.7223958927552766</v>
       </c>
     </row>
-    <row r="213" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B213">
         <v>0.54948494678732007</v>
       </c>
@@ -2112,7 +2116,7 @@
         <v>0.7275613226338854</v>
       </c>
     </row>
-    <row r="214" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B214">
         <v>0.54767309875141879</v>
       </c>
@@ -2120,7 +2124,7 @@
         <v>0.73639103291713948</v>
       </c>
     </row>
-    <row r="215" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B215">
         <v>0.54777758807125387</v>
       </c>
@@ -2128,7 +2132,7 @@
         <v>0.74823629844630357</v>
       </c>
     </row>
-    <row r="216" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B216">
         <v>0.54894323844435544</v>
       </c>
@@ -2136,7 +2140,7 @@
         <v>0.75961910762357521</v>
       </c>
     </row>
-    <row r="217" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B217">
         <v>0.55053974484789014</v>
       </c>
@@ -2144,7 +2148,7 @@
         <v>0.77056745367430579</v>
       </c>
     </row>
-    <row r="218" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B218">
         <v>0.55205304175875314</v>
       </c>
@@ -2152,7 +2156,7 @@
         <v>0.78203675700825881</v>
       </c>
     </row>
-    <row r="219" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B219">
         <v>0.55319398091223138</v>
       </c>
@@ -2160,7 +2164,7 @@
         <v>0.79426254464547097</v>
       </c>
     </row>
-    <row r="220" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B220">
         <v>0.5524479624743478</v>
       </c>
@@ -2168,7 +2172,7 @@
         <v>0.80221577250073306</v>
       </c>
     </row>
-    <row r="221" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B221">
         <v>0.55012868507253154</v>
       </c>
@@ -2176,7 +2180,7 @@
         <v>0.80584990641085641</v>
       </c>
     </row>
-    <row r="222" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B222">
         <v>0.54820118756549074</v>
       </c>
@@ -2184,7 +2188,7 @@
         <v>0.80532541623006171</v>
       </c>
     </row>
-    <row r="223" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B223">
         <v>0.54773753037842832</v>
       </c>
@@ -2192,7 +2196,7 @@
         <v>0.80054681171160735</v>
       </c>
     </row>
-    <row r="224" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B224">
         <v>0.54788853777650104</v>
       </c>
@@ -2200,7 +2204,7 @@
         <v>0.79277104280379207</v>
       </c>
     </row>
-    <row r="225" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B225">
         <v>0.54520015989949167</v>
       </c>
@@ -2208,7 +2212,7 @@
         <v>0.7851584718177147</v>
       </c>
     </row>
-    <row r="226" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B226">
         <v>0.54058349415370643</v>
       </c>
@@ -2216,7 +2220,7 @@
         <v>0.77851458735384271</v>
       </c>
     </row>
-    <row r="227" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B227">
         <v>0.53468811741462041</v>
       </c>
@@ -2224,7 +2228,7 @@
         <v>0.77515664690939889</v>
       </c>
     </row>
-    <row r="228" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B228">
         <v>0.52789482555199729</v>
       </c>
@@ -2232,7 +2236,7 @@
         <v>0.77544693522107977</v>
       </c>
     </row>
-    <row r="229" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B229">
         <v>0.5222508687366888</v>
       </c>
@@ -2240,7 +2244,7 @@
         <v>0.77962392108508027</v>
       </c>
     </row>
-    <row r="230" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B230">
         <v>0.52455596278545258</v>
       </c>
@@ -2248,7 +2252,7 @@
         <v>0.78999097829151399</v>
       </c>
     </row>
-    <row r="231" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B231">
         <v>0.53300593878483327</v>
       </c>
@@ -2256,7 +2260,7 @@
         <v>0.80188042485153033</v>
       </c>
     </row>
-    <row r="232" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B232">
         <v>0.54032443626323057</v>
       </c>
@@ -2264,7 +2268,7 @@
         <v>0.80556776346065351</v>
       </c>
     </row>
-    <row r="233" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B233">
         <v>0.54625144175317186</v>
       </c>
@@ -2272,7 +2276,7 @@
         <v>0.80288869665513263</v>
       </c>
     </row>
-    <row r="234" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B234">
         <v>0.5499971216395142</v>
       </c>
@@ -2280,7 +2284,7 @@
         <v>0.79624719359852636</v>
       </c>
     </row>
-    <row r="235" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B235">
         <v>0.54996282102613969</v>
       </c>
@@ -2288,7 +2292,7 @@
         <v>0.78673053823714467</v>
       </c>
     </row>
-    <row r="236" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B236">
         <v>0.546875</v>
       </c>
@@ -2296,7 +2300,7 @@
         <v>0.77447860054347828</v>
       </c>
     </row>
-    <row r="237" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B237">
         <v>0.54506582648812874</v>
       </c>
@@ -2304,7 +2308,7 @@
         <v>0.76481996174187006</v>
       </c>
     </row>
-    <row r="238" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B238">
         <v>0.54429244225162599</v>
       </c>
@@ -2312,7 +2316,7 @@
         <v>0.75634166853554607</v>
       </c>
     </row>
-    <row r="239" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B239">
         <v>0.54299932900917014</v>
       </c>
@@ -2320,7 +2324,7 @@
         <v>0.74811787072243341</v>
       </c>
     </row>
-    <row r="240" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B240">
         <v>0.54021066711252308</v>
       </c>
@@ -2328,7 +2332,7 @@
         <v>0.73903973694476965</v>
       </c>
     </row>
-    <row r="241" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B241">
         <v>0.53642825410928474</v>
       </c>
@@ -2336,7 +2340,7 @@
         <v>0.7301338294091515</v>
       </c>
     </row>
-    <row r="242" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B242">
         <v>0.53473380015560745</v>
       </c>
@@ -2344,7 +2348,7 @@
         <v>0.72778259419806601</v>
       </c>
     </row>
-    <row r="243" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B243">
         <v>0.53396110770602323</v>
       </c>
@@ -2352,7 +2356,7 @@
         <v>0.73442190895414272</v>
       </c>
     </row>
-    <row r="244" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B244">
         <v>0.53385853167951725</v>
       </c>
@@ -2360,7 +2364,7 @@
         <v>0.74655659850262601</v>
       </c>
     </row>
-    <row r="245" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B245">
         <v>0.53435627485019888</v>
       </c>
@@ -2368,7 +2372,7 @@
         <v>0.75814526516212144</v>
       </c>
     </row>
-    <row r="246" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B246">
         <v>0.5356761915455005</v>
       </c>
@@ -2376,7 +2380,7 @@
         <v>0.76547409195531357</v>
       </c>
     </row>
-    <row r="247" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B247">
         <v>0.53824905575286097</v>
       </c>
@@ -2384,7 +2388,7 @@
         <v>0.77026495292857566</v>
       </c>
     </row>
-    <row r="248" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B248">
         <v>0.54195962803356779</v>
       </c>
@@ -2392,7 +2396,7 @@
         <v>0.77500567022000466</v>
       </c>
     </row>
-    <row r="249" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B249">
         <v>0.54018437871161129</v>
       </c>
@@ -2400,7 +2404,7 @@
         <v>0.77177704880945641</v>
       </c>
     </row>
-    <row r="250" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B250">
         <v>0.53275158024277003</v>
       </c>
@@ -2408,7 +2412,7 @@
         <v>0.76000559377971688</v>
       </c>
     </row>
-    <row r="251" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B251">
         <v>0.52384105960264904</v>
       </c>
@@ -2416,7 +2420,7 @@
         <v>0.74431070640176611</v>
       </c>
     </row>
-    <row r="252" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B252">
         <v>0.52059308072487631</v>
       </c>
@@ -2424,7 +2428,7 @@
         <v>0.73335475013728713</v>
       </c>
     </row>
-    <row r="253" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B253">
         <v>0.52281746031746035</v>
       </c>
@@ -2432,7 +2436,7 @@
         <v>0.72819058641975321</v>
       </c>
     </row>
-    <row r="254" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B254">
         <v>0.52853805073431237</v>
       </c>
@@ -2440,7 +2444,7 @@
         <v>0.7291967067200712</v>
       </c>
     </row>
-    <row r="255" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B255">
         <v>0.53711642599277976</v>
       </c>
@@ -2448,7 +2452,7 @@
         <v>0.73822314981949444</v>
       </c>
     </row>
-    <row r="256" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B256">
         <v>0.54394977168949776</v>
       </c>
@@ -2456,7 +2460,7 @@
         <v>0.74825913242009134</v>
       </c>
     </row>
-    <row r="257" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B257">
         <v>0.54355659783789967</v>
       </c>
@@ -2464,7 +2468,7 @@
         <v>0.75035806211748568</v>
       </c>
     </row>
-    <row r="258" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B258">
         <v>0.53728456856834073</v>
       </c>
@@ -2472,7 +2476,7 @@
         <v>0.74332119902167104</v>
       </c>
     </row>
-    <row r="259" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B259">
         <v>0.53126952570292529</v>
       </c>
@@ -2480,7 +2484,7 @@
         <v>0.73429650667424029</v>
       </c>
     </row>
-    <row r="260" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B260">
         <v>0.52530997611193264</v>
       </c>
@@ -2488,7 +2492,7 @@
         <v>0.72391878057103864</v>
       </c>
     </row>
-    <row r="261" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B261">
         <v>0.51970302684180469</v>
       </c>
@@ -2496,7 +2500,7 @@
         <v>0.71466876070816687</v>
       </c>
     </row>
-    <row r="262" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B262">
         <v>0.51440068985340615</v>
       </c>
@@ -2504,7 +2508,7 @@
         <v>0.70859902270767461</v>
       </c>
     </row>
-    <row r="263" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B263">
         <v>0.50912673118154961</v>
       </c>
@@ -2512,7 +2516,7 @@
         <v>0.70585327693110045</v>
       </c>
     </row>
-    <row r="264" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B264">
         <v>0.50565597667638484</v>
       </c>
@@ -2520,7 +2524,7 @@
         <v>0.70304489795918368</v>
       </c>
     </row>
-    <row r="265" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B265">
         <v>0.50290101388970276</v>
       </c>
@@ -2528,7 +2532,7 @@
         <v>0.70015999531149264</v>
       </c>
     </row>
-    <row r="266" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B266">
         <v>0.50052984811020851</v>
       </c>
@@ -2536,7 +2540,7 @@
         <v>0.69776462969504305</v>
       </c>
     </row>
-    <row r="267" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B267">
         <v>0.49840350047303694</v>
       </c>
@@ -2544,7 +2548,7 @@
         <v>0.69687559129612109</v>
       </c>
     </row>
-    <row r="268" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="268" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B268">
         <v>0.49776878681501757</v>
       </c>
@@ -2552,7 +2556,7 @@
         <v>0.6990242161004343</v>
       </c>
     </row>
-    <row r="269" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B269">
         <v>0.50399322362052268</v>
       </c>
@@ -2560,7 +2564,7 @@
         <v>0.71038661665053238</v>
       </c>
     </row>
-    <row r="270" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="270" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B270">
         <v>0.51619910625620646</v>
       </c>
@@ -2568,7 +2572,7 @@
         <v>0.73007075471698102</v>
       </c>
     </row>
-    <row r="271" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B271">
         <v>0.52840368137099336</v>
       </c>
@@ -2576,7 +2580,7 @@
         <v>0.75063598857505553</v>
       </c>
     </row>
-    <row r="272" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="272" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B272">
         <v>0.54010349288486426</v>
       </c>
@@ -2584,7 +2588,7 @@
         <v>0.77184993531694701</v>
       </c>
     </row>
-    <row r="273" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="273" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B273">
         <v>0.55030128373067855</v>
       </c>
@@ -2592,7 +2596,7 @@
         <v>0.7908704479958083</v>
       </c>
     </row>
-    <row r="274" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="274" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B274">
         <v>0.55701093719300554</v>
       </c>
@@ -2600,7 +2604,7 @@
         <v>0.80118016896980826</v>
       </c>
     </row>
-    <row r="275" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="275" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B275">
         <v>0.56110534509600418</v>
       </c>
@@ -2608,7 +2612,7 @@
         <v>0.8034723663726</v>
       </c>
     </row>
-    <row r="276" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="276" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B276">
         <v>0.55638426722764067</v>
       </c>
@@ -2616,7 +2620,7 @@
         <v>0.79828902913240263</v>
       </c>
     </row>
-    <row r="277" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="277" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B277">
         <v>0.54606083271004735</v>
       </c>
@@ -2624,7 +2628,7 @@
         <v>0.78721515831463484</v>
       </c>
     </row>
-    <row r="278" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="278" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B278">
         <v>0.53454700959130075</v>
       </c>
@@ -2632,7 +2636,7 @@
         <v>0.77568391471684295</v>
       </c>
     </row>
-    <row r="279" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="279" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B279">
         <v>0.52498792853693865</v>
       </c>
@@ -2640,7 +2644,7 @@
         <v>0.7676170931916948</v>
       </c>
     </row>
-    <row r="280" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="280" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B280">
         <v>0.51686067442697714</v>
       </c>
@@ -2648,7 +2652,7 @@
         <v>0.76248049921996897</v>
       </c>
     </row>
-    <row r="281" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="281" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B281">
         <v>0.51350378105869643</v>
       </c>
@@ -2656,7 +2660,7 @@
         <v>0.76033969511463229</v>
       </c>
     </row>
-    <row r="282" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="282" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B282">
         <v>0.51304767070451396</v>
       </c>
@@ -2664,7 +2668,7 @@
         <v>0.75942867474236131</v>
       </c>
     </row>
-    <row r="283" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="283" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B283">
         <v>0.51346118942464769</v>
       </c>
@@ -2672,7 +2676,7 @@
         <v>0.75693266380301294</v>
       </c>
     </row>
-    <row r="284" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="284" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B284">
         <v>0.5139410837677294</v>
       </c>
@@ -2680,7 +2684,7 @@
         <v>0.75307128136743839</v>
       </c>
     </row>
-    <row r="285" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="285" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B285">
         <v>0.51474335638878776</v>
       </c>
@@ -2688,7 +2692,7 @@
         <v>0.74931258342434159</v>
       </c>
     </row>
-    <row r="286" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="286" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B286">
         <v>0.51793557833089299</v>
       </c>
@@ -2696,7 +2700,7 @@
         <v>0.74988286969253282</v>
       </c>
     </row>
-    <row r="287" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="287" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B287">
         <v>0.52282795963573714</v>
       </c>
@@ -2704,7 +2708,7 @@
         <v>0.7550707605217819</v>
       </c>
     </row>
-    <row r="288" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="288" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B288">
         <v>0.52624087139497466</v>
       </c>
@@ -2712,7 +2716,7 @@
         <v>0.76226946404257945</v>
       </c>
     </row>
-    <row r="289" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="289" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B289">
         <v>0.52815196474020731</v>
       </c>
@@ -2720,7 +2724,7 @@
         <v>0.77200322800918741</v>
       </c>
     </row>
-    <row r="290" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="290" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B290">
         <v>0.52941542288557208</v>
       </c>
@@ -2728,7 +2732,7 @@
         <v>0.7828202736318407</v>
       </c>
     </row>
-    <row r="291" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="291" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B291">
         <v>0.53119151590767311</v>
       </c>
@@ -2736,7 +2740,7 @@
         <v>0.79019401122894561</v>
       </c>
     </row>
-    <row r="292" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="292" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B292">
         <v>0.53314969010204716</v>
       </c>
@@ -2744,7 +2748,7 @@
         <v>0.7886013898453641</v>
       </c>
     </row>
-    <row r="293" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="293" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B293">
         <v>0.53642592243384246</v>
       </c>
@@ -2752,7 +2756,7 @@
         <v>0.77789490225658442</v>
       </c>
     </row>
-    <row r="294" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="294" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B294">
         <v>0.54081697076835666</v>
       </c>
@@ -2760,7 +2764,7 @@
         <v>0.76358419092114416</v>
       </c>
     </row>
-    <row r="295" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="295" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B295">
         <v>0.54424610710216481</v>
       </c>
@@ -2768,7 +2772,7 @@
         <v>0.75285099379668308</v>
       </c>
     </row>
-    <row r="296" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="296" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B296">
         <v>0.54415666456096012</v>
       </c>
@@ -2776,7 +2780,7 @@
         <v>0.74769993682880598</v>
       </c>
     </row>
-    <row r="297" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="297" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B297">
         <v>0.54120603015075375</v>
       </c>
@@ -2784,7 +2788,7 @@
         <v>0.74768530150753765</v>
       </c>
     </row>
-    <row r="298" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="298" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B298">
         <v>0.54300296137609483</v>
       </c>
@@ -2792,7 +2796,7 @@
         <v>0.75752630584084191</v>
       </c>
     </row>
-    <row r="299" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="299" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B299">
         <v>0.54792169823312575</v>
       </c>
@@ -2800,7 +2804,7 @@
         <v>0.76745074361255872</v>
       </c>
     </row>
-    <row r="300" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="300" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B300">
         <v>0.5533350469091376</v>
       </c>
@@ -2808,7 +2812,7 @@
         <v>0.77259542475260246</v>
       </c>
     </row>
-    <row r="301" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="301" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B301">
         <v>0.55746118365490804</v>
       </c>
@@ -2816,7 +2820,7 @@
         <v>0.77526343142987075</v>
       </c>
     </row>
-    <row r="302" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="302" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B302">
         <v>0.55977690288713911</v>
       </c>
@@ -2824,7 +2828,7 @@
         <v>0.78122506561679783</v>
       </c>
     </row>
-    <row r="303" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="303" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B303">
         <v>0.55296902742158205</v>
       </c>
@@ -2832,7 +2836,7 @@
         <v>0.78940816729137897</v>
       </c>
     </row>
-    <row r="304" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="304" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B304">
         <v>0.54014024510125169</v>
       </c>
@@ -2840,7 +2844,7 @@
         <v>0.79804050068811849</v>
       </c>
     </row>
-    <row r="305" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="305" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B305">
         <v>0.52967378488143579</v>
       </c>
@@ -2848,7 +2852,7 @@
         <v>0.81166579326608146</v>
       </c>
     </row>
-    <row r="306" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="306" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B306">
         <v>0.52355883127138714</v>
       </c>
@@ -2856,7 +2860,7 @@
         <v>0.83197617794156364</v>
       </c>
     </row>
-    <row r="307" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="307" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B307">
         <v>0.52025416997617158</v>
       </c>
@@ -2864,7 +2868,7 @@
         <v>0.85728554408260504</v>
       </c>
     </row>
-    <row r="308" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="308" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B308">
         <v>0.51532252772491638</v>
       </c>
@@ -2872,7 +2876,7 @@
         <v>0.87065096134916986</v>
       </c>
     </row>
-    <row r="309" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="309" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B309">
         <v>0.50943396226415094</v>
       </c>
@@ -2880,7 +2884,7 @@
         <v>0.87025436280507418</v>
       </c>
     </row>
-    <row r="310" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="310" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B310">
         <v>0.51261688228512881</v>
       </c>
@@ -2888,7 +2892,7 @@
         <v>0.87352312027667478</v>
       </c>
     </row>
-    <row r="311" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="311" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B311">
         <v>0.52382794866834337</v>
       </c>
@@ -2896,7 +2900,7 @@
         <v>0.87975688398787655</v>
       </c>
     </row>
-    <row r="312" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="312" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B312">
         <v>0.53812479581836004</v>
       </c>
@@ -2904,7 +2908,7 @@
         <v>0.8890532505717087</v>
       </c>
     </row>
-    <row r="313" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="313" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B313">
         <v>0.54794158461640119</v>
       </c>
@@ -2912,7 +2916,7 @@
         <v>0.89734355382277142</v>
       </c>
     </row>
-    <row r="314" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="314" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B314">
         <v>0.55431661881551719</v>
       </c>
@@ -2920,7 +2924,7 @@
         <v>0.90671229218134464</v>
       </c>
     </row>
-    <row r="315" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="315" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B315">
         <v>0.55640203154236834</v>
       </c>
@@ -2928,7 +2932,7 @@
         <v>0.90934108527131785</v>
       </c>
     </row>
-    <row r="316" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="316" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B316">
         <v>0.55545218951425335</v>
       </c>
@@ -2936,7 +2940,7 @@
         <v>0.90698252375573141</v>
       </c>
     </row>
-    <row r="317" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="317" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B317">
         <v>0.5572145877378436</v>
       </c>
@@ -2944,7 +2948,7 @@
         <v>0.90568313953488389</v>
       </c>
     </row>
-    <row r="318" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="318" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B318">
         <v>0.56685163165543673</v>
       </c>
@@ -2952,7 +2956,7 @@
         <v>0.91103117981239279</v>
       </c>
     </row>
-    <row r="319" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="319" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B319">
         <v>0.58297928836962287</v>
       </c>
@@ -2960,7 +2964,7 @@
         <v>0.92219397238449263</v>
       </c>
     </row>
-    <row r="320" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="320" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B320">
         <v>0.58411519416210578</v>
       </c>
@@ -2968,7 +2972,7 @@
         <v>0.91104052645295797</v>
       </c>
     </row>
-    <row r="321" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="321" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B321">
         <v>0.57765977621847142</v>
       </c>
@@ -2976,7 +2980,7 @@
         <v>0.88765029395031281</v>
       </c>
     </row>
-    <row r="322" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="322" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B322">
         <v>0.56843524077931618</v>
       </c>
@@ -2984,7 +2988,7 @@
         <v>0.86162847690234035</v>
       </c>
     </row>
-    <row r="323" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="323" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B323">
         <v>0.55873242792470812</v>
       </c>
@@ -2992,7 +2996,7 @@
         <v>0.83712115796997866</v>
       </c>
     </row>
-    <row r="324" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="324" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B324">
         <v>0.54882721783557831</v>
       </c>
@@ -3000,7 +3004,7 @@
         <v>0.81434393869019972</v>
       </c>
     </row>
-    <row r="325" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="325" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B325">
         <v>0.54174259681093406</v>
       </c>
@@ -3008,7 +3012,7 @@
         <v>0.79627619589977228</v>
       </c>
     </row>
-    <row r="326" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="326" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B326">
         <v>0.53591438816674131</v>
       </c>
@@ -3016,7 +3020,7 @@
         <v>0.78011317794710888</v>
       </c>
     </row>
-    <row r="327" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="327" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B327">
         <v>0.53339636282742897</v>
       </c>
@@ -3024,7 +3028,7 @@
         <v>0.77061787442300211</v>
       </c>
     </row>
-    <row r="328" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="328" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B328">
         <v>0.53385634006565408</v>
       </c>
@@ -3032,7 +3036,7 @@
         <v>0.7676375674623046</v>
       </c>
     </row>
-    <row r="329" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="329" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B329">
         <v>0.535670356703567</v>
       </c>
@@ -3040,7 +3044,7 @@
         <v>0.76894554400089454</v>
       </c>
     </row>
-    <row r="330" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="330" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B330">
         <v>0.53654839434089374</v>
       </c>
@@ -3048,7 +3052,7 @@
         <v>0.77071524814731629</v>
       </c>
     </row>
-    <row r="331" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="331" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B331">
         <v>0.53686999661743151</v>
       </c>
@@ -3056,7 +3060,7 @@
         <v>0.77321795016349082</v>
       </c>
     </row>
-    <row r="332" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="332" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B332">
         <v>0.53554315350357973</v>
       </c>
@@ -3064,7 +3068,7 @@
         <v>0.77228141383392546</v>
       </c>
     </row>
-    <row r="333" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="333" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B333">
         <v>0.53292504775817517</v>
       </c>
@@ -3072,7 +3076,7 @@
         <v>0.76768738060456243</v>
       </c>
     </row>
-    <row r="334" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="334" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B334">
         <v>0.53064082455747252</v>
       </c>
@@ -3080,7 +3084,7 @@
         <v>0.7614138471879901</v>
       </c>
     </row>
-    <row r="335" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="335" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B335">
         <v>0.53066606812187878</v>
       </c>
@@ -3088,7 +3092,7 @@
         <v>0.75702990853487484</v>
       </c>
     </row>
-    <row r="336" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="336" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B336">
         <v>0.5322316846201568</v>
       </c>
@@ -3096,7 +3100,7 @@
         <v>0.75543567762675556</v>
       </c>
     </row>
-    <row r="337" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="337" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B337">
         <v>0.53467879476975555</v>
       </c>
@@ -3104,7 +3108,7 @@
         <v>0.75786355884025014</v>
       </c>
     </row>
-    <row r="338" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="338" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B338">
         <v>0.53778135048231512</v>
       </c>
@@ -3112,7 +3116,7 @@
         <v>0.76400206706476814</v>
       </c>
     </row>
-    <row r="339" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="339" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B339">
         <v>0.53925883034163291</v>
       </c>
@@ -3120,7 +3124,7 @@
         <v>0.77088071800810665</v>
       </c>
     </row>
-    <row r="340" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="340" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B340">
         <v>0.53753998255306779</v>
       </c>
@@ -3128,7 +3132,7 @@
         <v>0.77574934574004062</v>
       </c>
     </row>
-    <row r="341" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="341" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B341">
         <v>0.5336051252184042</v>
       </c>
@@ -3136,7 +3140,7 @@
         <v>0.77915958066394864</v>
       </c>
     </row>
-    <row r="342" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="342" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B342">
         <v>0.52674754477180818</v>
       </c>
@@ -3144,7 +3148,7 @@
         <v>0.77501386481802426</v>
       </c>
     </row>
-    <row r="343" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="343" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B343">
         <v>0.51855864074348601</v>
       </c>
@@ -3152,7 +3156,7 @@
         <v>0.76361024003649025</v>
       </c>
     </row>
-    <row r="344" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="344" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B344">
         <v>0.51224593209841784</v>
       </c>
@@ -3160,7 +3164,7 @@
         <v>0.74628568211249358</v>
       </c>
     </row>
-    <row r="345" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="345" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B345">
         <v>0.50858225590726702</v>
       </c>
@@ -3168,7 +3172,7 @@
         <v>0.72388709317877842</v>
       </c>
     </row>
-    <row r="346" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="346" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B346">
         <v>0.50685916583692892</v>
       </c>
@@ -3176,7 +3180,7 @@
         <v>0.70080097355902216</v>
       </c>
     </row>
-    <row r="347" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="347" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B347">
         <v>0.50680987709002323</v>
       </c>
@@ -3184,7 +3188,7 @@
         <v>0.68847193001882401</v>
       </c>
     </row>
-    <row r="348" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="348" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B348">
         <v>0.5085975882090219</v>
       </c>
@@ -3192,7 +3196,7 @@
         <v>0.68823246985261277</v>
       </c>
     </row>
-    <row r="349" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="349" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B349">
         <v>0.51377082624957493</v>
       </c>
@@ -3200,7 +3204,7 @@
         <v>0.69786920548566245</v>
       </c>
     </row>
-    <row r="350" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="350" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B350">
         <v>0.52237078196446141</v>
       </c>
@@ -3208,7 +3212,7 @@
         <v>0.71498003125542631</v>
       </c>
     </row>
-    <row r="351" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="351" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B351">
         <v>0.53167099976364929</v>
       </c>
@@ -3216,7 +3220,7 @@
         <v>0.73499054597021973</v>
       </c>
     </row>
-    <row r="352" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="352" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B352">
         <v>0.53512838801711848</v>
       </c>
@@ -3224,7 +3228,7 @@
         <v>0.74765275796481223</v>
       </c>
     </row>
-    <row r="353" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="353" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B353">
         <v>0.53271634048573446</v>
       </c>
@@ -3232,7 +3236,7 @@
         <v>0.75156979485970288</v>
       </c>
     </row>
-    <row r="354" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="354" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B354">
         <v>0.53066369606003749</v>
       </c>
@@ -3240,7 +3244,7 @@
         <v>0.75585952157598502</v>
       </c>
     </row>
-    <row r="355" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="355" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B355">
         <v>0.52874839312843291</v>
       </c>
@@ -3248,7 +3252,7 @@
         <v>0.75521327568072927</v>
       </c>
     </row>
-    <row r="356" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="356" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B356">
         <v>0.52776154295733491</v>
       </c>
@@ -3256,7 +3260,7 @@
         <v>0.75084161309175923</v>
       </c>
     </row>
-    <row r="357" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="357" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B357">
         <v>0.52855799741450227</v>
       </c>
@@ -3264,7 +3268,7 @@
         <v>0.74608649665060522</v>
       </c>
     </row>
-    <row r="358" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="358" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B358">
         <v>0.53034973325429768</v>
       </c>
@@ -3272,7 +3276,7 @@
         <v>0.74284825133372867</v>
       </c>
     </row>
-    <row r="359" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="359" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B359">
         <v>0.53526598924088464</v>
       </c>
@@ -3280,7 +3284,7 @@
         <v>0.74163538553496711</v>
       </c>
     </row>
-    <row r="360" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="360" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B360">
         <v>0.54211858279103387</v>
       </c>
@@ -3288,7 +3292,7 @@
         <v>0.74340503735839958</v>
       </c>
     </row>
-    <row r="361" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="361" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B361">
         <v>0.54503199323916451</v>
       </c>
@@ -3296,7 +3300,7 @@
         <v>0.74330435832427866</v>
       </c>
     </row>
-    <row r="362" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="362" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B362">
         <v>0.5414593201031237</v>
       </c>
@@ -3304,7 +3308,7 @@
         <v>0.7382840697883567</v>
       </c>
     </row>
-    <row r="363" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="363" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B363">
         <v>0.53370054489457475</v>
       </c>
@@ -3312,7 +3316,7 @@
         <v>0.72890547263681582</v>
       </c>
     </row>
-    <row r="364" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="364" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B364">
         <v>0.52960254747022051</v>
       </c>
@@ -3320,7 +3324,7 @@
         <v>0.72401757282698409</v>
       </c>
     </row>
-    <row r="365" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="365" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B365">
         <v>0.52748289690964845</v>
       </c>
@@ -3328,7 +3332,7 @@
         <v>0.72176456711488557</v>
       </c>
     </row>
-    <row r="366" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="366" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B366">
         <v>0.52705659707847885</v>
       </c>
@@ -3336,7 +3340,7 @@
         <v>0.72221479685374645</v>
       </c>
     </row>
-    <row r="367" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="367" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B367">
         <v>0.52780087917310214</v>
       </c>
@@ -3344,7 +3348,7 @@
         <v>0.72625341570630864</v>
       </c>
     </row>
-    <row r="368" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="368" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B368">
         <v>0.52924308501105199</v>
       </c>
@@ -3352,7 +3356,7 @@
         <v>0.73361192424876043</v>
       </c>
     </row>
-    <row r="369" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="369" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B369">
         <v>0.53055822906641004</v>
       </c>
@@ -3360,7 +3364,7 @@
         <v>0.74404054379210793</v>
       </c>
     </row>
-    <row r="370" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="370" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B370">
         <v>0.53176912816781863</v>
       </c>
@@ -3368,7 +3372,7 @@
         <v>0.75627682793743189</v>
       </c>
     </row>
-    <row r="371" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="371" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B371">
         <v>0.53133215137250112</v>
       </c>
@@ -3376,7 +3380,7 @@
         <v>0.767375435593324</v>
       </c>
     </row>
-    <row r="372" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="372" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B372">
         <v>0.52934286771051664</v>
       </c>
@@ -3384,7 +3388,7 @@
         <v>0.77505054863765266</v>
       </c>
     </row>
-    <row r="373" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="373" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B373">
         <v>0.52771908017402114</v>
       </c>
@@ -3392,7 +3396,7 @@
         <v>0.77870913610938475</v>
       </c>
     </row>
-    <row r="374" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="374" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B374">
         <v>0.52913898984835195</v>
       </c>
@@ -3400,7 +3404,7 @@
         <v>0.77877992229602699</v>
       </c>
     </row>
-    <row r="375" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="375" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B375">
         <v>0.53340919147860166</v>
       </c>
@@ -3408,7 +3412,7 @@
         <v>0.77575320816739346</v>
       </c>
     </row>
-    <row r="376" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="376" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B376">
         <v>0.53498282661239027</v>
       </c>
@@ -3416,7 +3420,7 @@
         <v>0.7696584404019845</v>
       </c>
     </row>
-    <row r="377" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="377" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B377">
         <v>0.53484954960710396</v>
       </c>
@@ -3424,7 +3428,7 @@
         <v>0.7639468472497285</v>
       </c>
     </row>
-    <row r="378" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="378" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B378">
         <v>0.53424833247819392</v>
       </c>
@@ -3432,7 +3436,7 @@
         <v>0.7614045664443303</v>
       </c>
     </row>
-    <row r="379" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="379" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B379">
         <v>0.53394306324874408</v>
       </c>
@@ -3440,7 +3444,7 @@
         <v>0.76283782043024606</v>
       </c>
     </row>
-    <row r="380" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="380" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B380">
         <v>0.53382923673997418</v>
       </c>
@@ -3448,7 +3452,7 @@
         <v>0.766173997412678</v>
       </c>
     </row>
-    <row r="381" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="381" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B381">
         <v>0.53508030431107345</v>
       </c>
@@ -3456,7 +3460,7 @@
         <v>0.77164575069900521</v>
       </c>
     </row>
-    <row r="382" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="382" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B382">
         <v>0.53704793669478779</v>
       </c>
@@ -3464,7 +3468,7 @@
         <v>0.77852331436792888</v>
       </c>
     </row>
-    <row r="383" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="383" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B383">
         <v>0.53690616411464465</v>
       </c>
@@ -3472,7 +3476,7 @@
         <v>0.78140753828032972</v>
       </c>
     </row>
-    <row r="384" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="384" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B384">
         <v>0.53399258343634115</v>
       </c>
@@ -3480,7 +3484,7 @@
         <v>0.77781471602368091</v>
       </c>
     </row>
-    <row r="385" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="385" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B385">
         <v>0.53051491912096416</v>
       </c>
@@ -3488,7 +3492,7 @@
         <v>0.76923503254495074</v>
       </c>
     </row>
-    <row r="386" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="386" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B386">
         <v>0.53673875377013414</v>
       </c>
@@ -3496,135 +3500,144 @@
         <v>0.76355323108515694</v>
       </c>
     </row>
-    <row r="387" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="387" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B387">
-        <v>0.54940052574212994</v>
+        <v>0.55606494746895896</v>
       </c>
       <c r="C387">
-        <v>0.76302814643841776</v>
-      </c>
-    </row>
-    <row r="388" spans="2:3" x14ac:dyDescent="0.25">
+        <v>0.76295065265838902</v>
+      </c>
+    </row>
+    <row r="388" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B388">
-        <v>0.55606494746895896</v>
+        <v>0.55614906051655877</v>
       </c>
       <c r="C388">
-        <v>0.76295065265838902</v>
-      </c>
-    </row>
-    <row r="389" spans="2:3" x14ac:dyDescent="0.25">
+        <v>0.76228680952680206</v>
+      </c>
+    </row>
+    <row r="389" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B389">
-        <v>0.55614906051655877</v>
+        <v>0.55082230740694949</v>
       </c>
       <c r="C389">
-        <v>0.76228680952680206</v>
-      </c>
-    </row>
-    <row r="390" spans="2:3" x14ac:dyDescent="0.25">
+        <v>0.76002967725979975</v>
+      </c>
+    </row>
+    <row r="390" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B390">
-        <v>0.55082230740694949</v>
+        <v>0.54030487804878047</v>
       </c>
       <c r="C390">
-        <v>0.76002967725979975</v>
-      </c>
-    </row>
-    <row r="391" spans="2:3" x14ac:dyDescent="0.25">
+        <v>0.75653963414634151</v>
+      </c>
+    </row>
+    <row r="391" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B391">
-        <v>0.54030487804878047</v>
+        <v>0.52522880539499028</v>
       </c>
       <c r="C391">
-        <v>0.75653963414634151</v>
-      </c>
-    </row>
-    <row r="392" spans="2:3" x14ac:dyDescent="0.25">
+        <v>0.74991570327552992</v>
+      </c>
+    </row>
+    <row r="392" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B392">
-        <v>0.52522880539499028</v>
+        <v>0.51625307937270926</v>
       </c>
       <c r="C392">
-        <v>0.74991570327552992</v>
-      </c>
-    </row>
-    <row r="393" spans="2:3" x14ac:dyDescent="0.25">
+        <v>0.74679324640990208</v>
+      </c>
+    </row>
+    <row r="393" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B393">
-        <v>0.51625307937270926</v>
+        <v>0.51181911613566289</v>
       </c>
       <c r="C393">
-        <v>0.74679324640990208</v>
-      </c>
-    </row>
-    <row r="394" spans="2:3" x14ac:dyDescent="0.25">
+        <v>0.74586240251496283</v>
+      </c>
+    </row>
+    <row r="394" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B394">
-        <v>0.51181911613566289</v>
+        <v>0.5125926833752068</v>
       </c>
       <c r="C394">
-        <v>0.74586240251496283</v>
-      </c>
-    </row>
-    <row r="395" spans="2:3" x14ac:dyDescent="0.25">
+        <v>0.74856179912984877</v>
+      </c>
+    </row>
+    <row r="395" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B395">
-        <v>0.5125926833752068</v>
+        <v>0.51953491279614927</v>
       </c>
       <c r="C395">
-        <v>0.74856179912984877</v>
-      </c>
-    </row>
-    <row r="396" spans="2:3" x14ac:dyDescent="0.25">
+        <v>0.75464712133525047</v>
+      </c>
+    </row>
+    <row r="396" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B396">
-        <v>0.51953491279614927</v>
+        <v>0.53157827312323858</v>
       </c>
       <c r="C396">
-        <v>0.75464712133525047</v>
-      </c>
-    </row>
-    <row r="397" spans="2:3" x14ac:dyDescent="0.25">
+        <v>0.76423264155777615</v>
+      </c>
+    </row>
+    <row r="397" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B397">
-        <v>0.53157827312323858</v>
+        <v>0.54005953921822425</v>
       </c>
       <c r="C397">
-        <v>0.76423264155777615</v>
-      </c>
-    </row>
-    <row r="398" spans="2:3" x14ac:dyDescent="0.25">
+        <v>0.7655203209940461</v>
+      </c>
+    </row>
+    <row r="398" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B398">
-        <v>0.54005953921822425</v>
+        <v>0.54563106796116501</v>
       </c>
       <c r="C398">
-        <v>0.7655203209940461</v>
-      </c>
-    </row>
-    <row r="399" spans="2:3" x14ac:dyDescent="0.25">
+        <v>0.76445242718446604</v>
+      </c>
+    </row>
+    <row r="399" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B399">
-        <v>0.54563106796116501</v>
+        <v>0.548478414720453</v>
       </c>
       <c r="C399">
-        <v>0.76445242718446604</v>
-      </c>
-    </row>
-    <row r="400" spans="2:3" x14ac:dyDescent="0.25">
+        <v>0.76413562375345823</v>
+      </c>
+    </row>
+    <row r="400" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B400">
-        <v>0.548478414720453</v>
+        <v>0.54872219743802175</v>
       </c>
       <c r="C400">
-        <v>0.76413562375345823</v>
-      </c>
-    </row>
-    <row r="401" spans="2:3" x14ac:dyDescent="0.25">
+        <v>0.76476260276591679</v>
+      </c>
+    </row>
+    <row r="401" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B401">
-        <v>0.54872219743802175</v>
+        <v>0.54667338075155802</v>
       </c>
       <c r="C401">
-        <v>0.76476260276591679</v>
-      </c>
-    </row>
-    <row r="402" spans="2:3" x14ac:dyDescent="0.25">
+        <v>0.76315541008371646</v>
+      </c>
+    </row>
+    <row r="402" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B402">
-        <v>0.54667338075155802</v>
+        <v>8</v>
       </c>
       <c r="C402">
-        <v>0.76315541008371646</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="403" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B403">
+        <v>5</v>
+      </c>
+      <c r="C403" s="2">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se añadieron las columnas de todos los datos clasificados y de los datos que quedan afuera de las regiones al archivo de Excel. Se agregaron a memorio en el programa todas las clasificaciones de matrices y sobrantes. Se grafica por color cada región.
</commit_message>
<xml_diff>
--- a/VerificacionCompuestos/DatosPruebaMvsN.xlsx
+++ b/VerificacionCompuestos/DatosPruebaMvsN.xlsx
@@ -1,24 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://comunidadunammx-my.sharepoint.com/personal/pamema_comunidad_unam_mx/Documents/Programación/Matemáticas/Matlab/Proyecto Ana/VerificacionCompuestos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{07B066D3-0FBB-4851-948D-1C1B43A25F31}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C633A1C-C859-41CB-97B6-F799DD8C782F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16389" windowHeight="10029" xr2:uid="{F0659778-C3FA-4246-A23C-D9F175EA623A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" xr2:uid="{F0659778-C3FA-4246-A23C-D9F175EA623A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -43,16 +48,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -86,10 +83,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,15 +400,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E623AF-0393-4572-BA98-9F6CD50E2EA0}">
-  <dimension ref="B1:C403"/>
+  <dimension ref="B1:C402"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A375" workbookViewId="0">
-      <selection activeCell="C404" sqref="C404"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,7 +416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -428,7 +424,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0.5535201807412834</v>
       </c>
@@ -436,7 +432,7 @@
         <v>0.79824204677291311</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>0.56169792694965448</v>
       </c>
@@ -444,7 +440,7 @@
         <v>0.82327307502467917</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>0.56733808490858373</v>
       </c>
@@ -452,7 +448,7 @@
         <v>0.83639231484350773</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>0.56739773287333661</v>
       </c>
@@ -460,7 +456,7 @@
         <v>0.83336619024149816</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>0.56311151625645695</v>
       </c>
@@ -468,7 +464,7 @@
         <v>0.81622910969310225</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>0.55514309663513361</v>
       </c>
@@ -476,7 +472,7 @@
         <v>0.79375943000838234</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>0.54544382188145091</v>
       </c>
@@ -484,7 +480,7 @@
         <v>0.77130875847832503</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>0.54110753003222967</v>
       </c>
@@ -492,7 +488,7 @@
         <v>0.75941634925285673</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>0.54243260703588414</v>
       </c>
@@ -500,7 +496,7 @@
         <v>0.75809420332413224</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>0.54660515732197779</v>
       </c>
@@ -508,7 +504,7 @@
         <v>0.75999704281996705</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>0.5477377983612397</v>
       </c>
@@ -516,7 +512,7 @@
         <v>0.75729485809286301</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>0.54664445502141834</v>
       </c>
@@ -524,7 +520,7 @@
         <v>0.75160102332222756</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>0.54247939764036279</v>
       </c>
@@ -532,7 +528,7 @@
         <v>0.74256358569988734</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>0.53625235404896432</v>
       </c>
@@ -540,7 +536,7 @@
         <v>0.73294197269303207</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>0.53064921404779997</v>
       </c>
@@ -548,7 +544,7 @@
         <v>0.72644363933851452</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>0.52886970722034299</v>
       </c>
@@ -556,7 +552,7 @@
         <v>0.72706812084451189</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>0.5301958491669102</v>
       </c>
@@ -564,7 +560,7 @@
         <v>0.73385676702718505</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>0.53471977440958762</v>
       </c>
@@ -572,7 +568,7 @@
         <v>0.74119551169075326</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>0.54161490683229807</v>
       </c>
@@ -580,7 +576,7 @@
         <v>0.74463531499556346</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>0.54857721157280626</v>
       </c>
@@ -588,7 +584,7 @@
         <v>0.74164602928920109</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>0.55403466826060965</v>
       </c>
@@ -596,7 +592,7 @@
         <v>0.73523789599521816</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>0.55881294964028771</v>
       </c>
@@ -604,7 +600,7 @@
         <v>0.73139688249400481</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>0.55683847161052247</v>
       </c>
@@ -612,7 +608,7 @@
         <v>0.7243149625044637</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>0.55120145702367662</v>
       </c>
@@ -620,7 +616,7 @@
         <v>0.71596028435462078</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>0.54431778527393282</v>
       </c>
@@ -628,7 +624,7 @@
         <v>0.71053158078399448</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>0.53700596030322323</v>
       </c>
@@ -636,7 +632,7 @@
         <v>0.70855216711995839</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>0.52996298010180465</v>
       </c>
@@ -644,7 +640,7 @@
         <v>0.7101457658491438</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>0.52833499035031284</v>
       </c>
@@ -652,7 +648,7 @@
         <v>0.72116439557868872</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>0.53039694838478968</v>
       </c>
@@ -660,7 +656,7 @@
         <v>0.74005662176659914</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>0.53475288851249181</v>
       </c>
@@ -668,7 +664,7 @@
         <v>0.75629363014941631</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>0.54058015267175563</v>
       </c>
@@ -676,7 +672,7 @@
         <v>0.7664030534351145</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>0.54587831207065751</v>
       </c>
@@ -684,7 +680,7 @@
         <v>0.76909102060843981</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>0.54735939223134411</v>
       </c>
@@ -692,7 +688,7 @@
         <v>0.76468570028182814</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>0.54590343818580833</v>
       </c>
@@ -700,7 +696,7 @@
         <v>0.75714459887832231</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>0.54147941212194828</v>
       </c>
@@ -708,7 +704,7 @@
         <v>0.75207032673387586</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>0.53520358700920989</v>
       </c>
@@ -716,7 +712,7 @@
         <v>0.75078829374697054</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>0.5315901489814534</v>
       </c>
@@ -724,7 +720,7 @@
         <v>0.75799331103678935</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>0.53514613392526822</v>
       </c>
@@ -732,7 +728,7 @@
         <v>0.77457084720680724</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>0.54480670997036007</v>
       </c>
@@ -740,7 +736,7 @@
         <v>0.79284543103991922</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>0.55123199999999994</v>
       </c>
@@ -748,7 +744,7 @@
         <v>0.79430015999999992</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>0.55533303184960281</v>
       </c>
@@ -756,7 +752,7 @@
         <v>0.78181536274953178</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>0.55765226444560123</v>
       </c>
@@ -764,7 +760,7 @@
         <v>0.76880921395106716</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>0.55883123689727454</v>
       </c>
@@ -772,7 +768,7 @@
         <v>0.76096698113207539</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>0.55881577212185152</v>
       </c>
@@ -780,7 +776,7 @@
         <v>0.75939074245021754</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>0.5574107202014178</v>
       </c>
@@ -788,7 +784,7 @@
         <v>0.76235208374743257</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>0.55483184899641103</v>
       </c>
@@ -796,7 +792,7 @@
         <v>0.76840821480792243</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>0.55442448436460412</v>
       </c>
@@ -804,7 +800,7 @@
         <v>0.77668928809048565</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>0.55667087681978322</v>
       </c>
@@ -812,7 +808,7 @@
         <v>0.78653460081100834</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>0.56088340628730604</v>
       </c>
@@ -820,7 +816,7 @@
         <v>0.79514060220188354</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>0.56504494976203068</v>
       </c>
@@ -828,7 +824,7 @@
         <v>0.79988696456901109</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>0.56937767533750416</v>
       </c>
@@ -836,7 +832,7 @@
         <v>0.80036088244978598</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>0.57145666710371057</v>
       </c>
@@ -844,7 +840,7 @@
         <v>0.79708732135833227</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>0.5715310380803339</v>
       </c>
@@ -852,7 +848,7 @@
         <v>0.78979786124152329</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>0.57036461369082325</v>
       </c>
@@ -860,7 +856,7 @@
         <v>0.77716080564730283</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>0.56901751909131748</v>
       </c>
@@ -868,7 +864,7 @@
         <v>0.75791631906564849</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>0.56737543636940657</v>
       </c>
@@ -876,7 +872,7 @@
         <v>0.73560583941605839</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>0.56312926020886744</v>
       </c>
@@ -884,7 +880,7 @@
         <v>0.71707272840973046</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>0.55746172292934881</v>
       </c>
@@ -892,7 +888,7 @@
         <v>0.70838590665928791</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>0.55149199417758366</v>
       </c>
@@ -900,7 +896,7 @@
         <v>0.70927583697234353</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>0.54585415788522917</v>
       </c>
@@ -908,7 +904,7 @@
         <v>0.71301017643162523</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>0.54065749143578334</v>
       </c>
@@ -916,7 +912,7 @@
         <v>0.71023919706713146</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>0.53372065165309057</v>
       </c>
@@ -924,7 +920,7 @@
         <v>0.69881827982750366</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>0.52594536562089944</v>
       </c>
@@ -932,7 +928,7 @@
         <v>0.68446856733866157</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>0.51442650201852291</v>
       </c>
@@ -940,7 +936,7 @@
         <v>0.6698883875563999</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67">
         <v>0.49861184948904247</v>
       </c>
@@ -948,7 +944,7 @@
         <v>0.65504046311063857</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68">
         <v>0.48049655821615578</v>
       </c>
@@ -956,7 +952,7 @@
         <v>0.64147437783138206</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69">
         <v>0.46610169491525427</v>
       </c>
@@ -964,7 +960,7 @@
         <v>0.63933684959108694</v>
       </c>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70">
         <v>0.45356176735798015</v>
       </c>
@@ -972,7 +968,7 @@
         <v>0.65007754733994594</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71">
         <v>0.45166676974457298</v>
       </c>
@@ -980,7 +976,7 @@
         <v>0.68136557610241844</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72">
         <v>0.46036251048184224</v>
       </c>
@@ -988,7 +984,7 @@
         <v>0.72933754757143776</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73">
         <v>0.47880839539607317</v>
       </c>
@@ -996,7 +992,7 @@
         <v>0.78719634394041993</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74">
         <v>0.50732394366197175</v>
       </c>
@@ -1004,7 +1000,7 @@
         <v>0.84151760563380296</v>
       </c>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75">
         <v>0.54566591586136737</v>
       </c>
@@ -1012,7 +1008,7 @@
         <v>0.88895589624355142</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76">
         <v>0.56731461483081369</v>
       </c>
@@ -1020,7 +1016,7 @@
         <v>0.89884233261339108</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77">
         <v>0.57519057519057515</v>
       </c>
@@ -1028,7 +1024,7 @@
         <v>0.87985169785169792</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78">
         <v>0.57558293587705356</v>
       </c>
@@ -1036,7 +1032,7 @@
         <v>0.85216878643349236</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79">
         <v>0.57404560594414555</v>
       </c>
@@ -1044,7 +1040,7 @@
         <v>0.82908147578785552</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80">
         <v>0.5711252653927813</v>
       </c>
@@ -1052,7 +1048,7 @@
         <v>0.80882228050455851</v>
       </c>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81">
         <v>0.56624374771257768</v>
       </c>
@@ -1060,7 +1056,7 @@
         <v>0.78672502134927413</v>
       </c>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82">
         <v>0.56007393715341969</v>
       </c>
@@ -1068,7 +1064,7 @@
         <v>0.76305229264802332</v>
       </c>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83">
         <v>0.5545731350275207</v>
       </c>
@@ -1076,7 +1072,7 @@
         <v>0.74100245930436814</v>
       </c>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84">
         <v>0.55059299971073183</v>
       </c>
@@ -1084,7 +1080,7 @@
         <v>0.72293549320219852</v>
       </c>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85">
         <v>0.54746871771323613</v>
       </c>
@@ -1092,7 +1088,7 @@
         <v>0.70832912409597071</v>
       </c>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86">
         <v>0.54403019213174741</v>
       </c>
@@ -1100,7 +1096,7 @@
         <v>0.69743938700823427</v>
       </c>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87">
         <v>0.54023972602739734</v>
       </c>
@@ -1108,7 +1104,7 @@
         <v>0.68807648401826504</v>
       </c>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88">
         <v>0.53767319363334487</v>
       </c>
@@ -1116,7 +1112,7 @@
         <v>0.68230447727012489</v>
       </c>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89">
         <v>0.53634894991922455</v>
       </c>
@@ -1124,7 +1120,7 @@
         <v>0.68156300484652665</v>
       </c>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90">
         <v>0.53647292250233425</v>
       </c>
@@ -1132,7 +1128,7 @@
         <v>0.68823587768440708</v>
       </c>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91">
         <v>0.54066559886100718</v>
       </c>
@@ -1140,7 +1136,7 @@
         <v>0.7057934389274485</v>
       </c>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92">
         <v>0.54834413029000417</v>
       </c>
@@ -1148,7 +1144,7 @@
         <v>0.72795362353938364</v>
       </c>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93">
         <v>0.5548189073050952</v>
       </c>
@@ -1156,7 +1152,7 @@
         <v>0.74392203806015955</v>
       </c>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94">
         <v>0.55996783571472764</v>
       </c>
@@ -1164,7 +1160,7 @@
         <v>0.75664439908455505</v>
       </c>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95">
         <v>0.56191538127981167</v>
       </c>
@@ -1172,7 +1168,7 @@
         <v>0.76922133432447493</v>
       </c>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96">
         <v>0.55739017928655044</v>
       </c>
@@ -1180,7 +1176,7 @@
         <v>0.77809438728359315</v>
       </c>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97">
         <v>0.54713763702801466</v>
       </c>
@@ -1188,7 +1184,7 @@
         <v>0.77728197320341053</v>
       </c>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98">
         <v>0.54262574595055413</v>
       </c>
@@ -1196,7 +1192,7 @@
         <v>0.77762574595055423</v>
       </c>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99">
         <v>0.54190698245183455</v>
       </c>
@@ -1204,7 +1200,7 @@
         <v>0.77590808688182611</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100">
         <v>0.54338663691583</v>
       </c>
@@ -1212,7 +1208,7 @@
         <v>0.7713778356266271</v>
       </c>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101">
         <v>0.54578411150696926</v>
       </c>
@@ -1220,7 +1216,7 @@
         <v>0.76493280830051891</v>
       </c>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102">
         <v>0.54910601863510444</v>
       </c>
@@ -1228,7 +1224,7 @@
         <v>0.76273860488541934</v>
       </c>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103">
         <v>0.55028952668680764</v>
       </c>
@@ -1236,7 +1232,7 @@
         <v>0.76506231117824774</v>
       </c>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104">
         <v>0.55008457056944193</v>
       </c>
@@ -1244,7 +1240,7 @@
         <v>0.76898264737204802</v>
       </c>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105">
         <v>0.54874027993779162</v>
       </c>
@@ -1252,7 +1248,7 @@
         <v>0.77204727838258169</v>
       </c>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106">
         <v>0.54643628509719222</v>
       </c>
@@ -1260,7 +1256,7 @@
         <v>0.77209564949089793</v>
       </c>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107">
         <v>0.5432468803523367</v>
       </c>
@@ -1268,7 +1264,7 @@
         <v>0.76596158551504789</v>
       </c>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108">
         <v>0.53978586202701051</v>
       </c>
@@ -1276,7 +1272,7 @@
         <v>0.75758547268524146</v>
       </c>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109">
         <v>0.53593939393939394</v>
       </c>
@@ -1284,7 +1280,7 @@
         <v>0.74886424242424254</v>
       </c>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110">
         <v>0.53271934076587502</v>
       </c>
@@ -1292,7 +1288,7 @@
         <v>0.74401539020843432</v>
       </c>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111">
         <v>0.53001579778830965</v>
       </c>
@@ -1300,7 +1296,7 @@
         <v>0.74454611738971932</v>
       </c>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112">
         <v>0.52912027407316775</v>
       </c>
@@ -1308,7 +1304,7 @@
         <v>0.74907500305885233</v>
       </c>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113">
         <v>0.5339962709757613</v>
       </c>
@@ -1316,7 +1312,7 @@
         <v>0.75986389061528903</v>
       </c>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114">
         <v>0.54320203303684889</v>
       </c>
@@ -1324,7 +1320,7 @@
         <v>0.77566010165184252</v>
       </c>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115">
         <v>0.55115106052767715</v>
       </c>
@@ -1332,7 +1328,7 @@
         <v>0.79123706673564398</v>
       </c>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116">
         <v>0.55765322844968856</v>
       </c>
@@ -1340,7 +1336,7 @@
         <v>0.80695640773516886</v>
       </c>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117">
         <v>0.56102868447082088</v>
       </c>
@@ -1348,7 +1344,7 @@
         <v>0.81763138806462243</v>
       </c>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118">
         <v>0.55934980664612954</v>
       </c>
@@ -1356,7 +1352,7 @@
         <v>0.81813724847610925</v>
       </c>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119">
         <v>0.55372700871248781</v>
       </c>
@@ -1364,7 +1360,7 @@
         <v>0.81016521458535007</v>
       </c>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120">
         <v>0.54976394028327158</v>
       </c>
@@ -1372,7 +1368,7 @@
         <v>0.80390519331376797</v>
       </c>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121">
         <v>0.54651162790697683</v>
       </c>
@@ -1380,7 +1376,7 @@
         <v>0.79853513650151675</v>
       </c>
     </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122">
         <v>0.54398496240601502</v>
       </c>
@@ -1388,7 +1384,7 @@
         <v>0.79471491228070179</v>
       </c>
     </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123">
         <v>0.54229072152134727</v>
       </c>
@@ -1396,7 +1392,7 @@
         <v>0.7930557454477658</v>
       </c>
     </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124">
         <v>0.540960364914011</v>
       </c>
@@ -1404,7 +1400,7 @@
         <v>0.79322628367133075</v>
       </c>
     </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125">
         <v>0.53434275596800773</v>
       </c>
@@ -1412,7 +1408,7 @@
         <v>0.79308993223029478</v>
       </c>
     </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126">
         <v>0.52488824453304328</v>
       </c>
@@ -1420,7 +1416,7 @@
         <v>0.79217953364745686</v>
       </c>
     </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127">
         <v>0.51801503759398493</v>
       </c>
@@ -1428,7 +1424,7 @@
         <v>0.79593383458646616</v>
       </c>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128">
         <v>0.51490645745322872</v>
       </c>
@@ -1436,7 +1432,7 @@
         <v>0.80373928786964388</v>
       </c>
     </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129">
         <v>0.51525114155251139</v>
       </c>
@@ -1444,7 +1440,7 @@
         <v>0.81206149162861496</v>
       </c>
     </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130">
         <v>0.52138066818433515</v>
       </c>
@@ -1452,7 +1448,7 @@
         <v>0.81747062080846589</v>
       </c>
     </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131">
         <v>0.53207124174866116</v>
       </c>
@@ -1460,7 +1456,7 @@
         <v>0.8215904844937103</v>
       </c>
     </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132">
         <v>0.54243658001879114</v>
       </c>
@@ -1468,7 +1464,7 @@
         <v>0.82087253366739765</v>
       </c>
     </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133">
         <v>0.55199198195940868</v>
       </c>
@@ -1476,7 +1472,7 @@
         <v>0.81602981708844913</v>
       </c>
     </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134">
         <v>0.5593241473907351</v>
       </c>
@@ -1484,7 +1480,7 @@
         <v>0.80746430575472294</v>
       </c>
     </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135">
         <v>0.56151945645460155</v>
       </c>
@@ -1492,7 +1488,7 @@
         <v>0.797696726374305</v>
       </c>
     </row>
-    <row r="136" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136">
         <v>0.55940775042651725</v>
       </c>
@@ -1500,7 +1496,7 @@
         <v>0.78889105532537174</v>
       </c>
     </row>
-    <row r="137" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137">
         <v>0.55667430362956716</v>
       </c>
@@ -1508,7 +1504,7 @@
         <v>0.7878415531170867</v>
       </c>
     </row>
-    <row r="138" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138">
         <v>0.55343693962940821</v>
       </c>
@@ -1516,7 +1512,7 @@
         <v>0.79293962940824858</v>
       </c>
     </row>
-    <row r="139" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139">
         <v>0.55060848916592464</v>
       </c>
@@ -1524,7 +1520,7 @@
         <v>0.79887800534283171</v>
       </c>
     </row>
-    <row r="140" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140">
         <v>0.54892812850646677</v>
       </c>
@@ -1532,7 +1528,7 @@
         <v>0.80414988484025285</v>
       </c>
     </row>
-    <row r="141" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141">
         <v>0.54792426202516753</v>
       </c>
@@ -1540,7 +1536,7 @@
         <v>0.80639127366811725</v>
       </c>
     </row>
-    <row r="142" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B142">
         <v>0.54624649204864362</v>
       </c>
@@ -1548,7 +1544,7 @@
         <v>0.80250818521983169</v>
       </c>
     </row>
-    <row r="143" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143">
         <v>0.54426629487626343</v>
       </c>
@@ -1556,7 +1552,7 @@
         <v>0.79106599279656098</v>
       </c>
     </row>
-    <row r="144" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144">
         <v>0.54204204204204209</v>
       </c>
@@ -1564,7 +1560,7 @@
         <v>0.77665049665049679</v>
       </c>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145">
         <v>0.53985861256394052</v>
       </c>
@@ -1572,7 +1568,7 @@
         <v>0.76270647738375774</v>
       </c>
     </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B146">
         <v>0.53808705612829322</v>
       </c>
@@ -1580,7 +1576,7 @@
         <v>0.75044730813287519</v>
       </c>
     </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B147">
         <v>0.54020618556701028</v>
       </c>
@@ -1588,7 +1584,7 @@
         <v>0.74239805269186721</v>
       </c>
     </row>
-    <row r="148" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B148">
         <v>0.54495349638305202</v>
       </c>
@@ -1596,7 +1592,7 @@
         <v>0.7401044896084511</v>
       </c>
     </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B149">
         <v>0.54781710745224022</v>
       </c>
@@ -1604,7 +1600,7 @@
         <v>0.74124490849635705</v>
       </c>
     </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B150">
         <v>0.54814941740918444</v>
       </c>
@@ -1612,7 +1608,7 @@
         <v>0.74401245145076533</v>
       </c>
     </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B151">
         <v>0.54697700823162088</v>
       </c>
@@ -1620,7 +1616,7 @@
         <v>0.74621061595231342</v>
       </c>
     </row>
-    <row r="152" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152">
         <v>0.54596336499321574</v>
       </c>
@@ -1628,7 +1624,7 @@
         <v>0.74868781094527348</v>
       </c>
     </row>
-    <row r="153" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B153">
         <v>0.54500846023688665</v>
       </c>
@@ -1636,7 +1632,7 @@
         <v>0.75231754089114489</v>
       </c>
     </row>
-    <row r="154" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B154">
         <v>0.54450586642599275</v>
       </c>
@@ -1644,7 +1640,7 @@
         <v>0.75844652527075807</v>
       </c>
     </row>
-    <row r="155" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="155" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B155">
         <v>0.54439608884869728</v>
       </c>
@@ -1652,7 +1648,7 @@
         <v>0.76494658904651558</v>
       </c>
     </row>
-    <row r="156" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B156">
         <v>0.54428086070215176</v>
       </c>
@@ -1660,7 +1656,7 @@
         <v>0.7680628539071348</v>
       </c>
     </row>
-    <row r="157" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B157">
         <v>0.5439569770733087</v>
       </c>
@@ -1668,7 +1664,7 @@
         <v>0.7664489102745542</v>
       </c>
     </row>
-    <row r="158" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="158" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B158">
         <v>0.54296037032855371</v>
       </c>
@@ -1676,7 +1672,7 @@
         <v>0.76219769673704418</v>
       </c>
     </row>
-    <row r="159" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="159" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B159">
         <v>0.54308108717717374</v>
       </c>
@@ -1684,7 +1680,7 @@
         <v>0.75976091124393808</v>
       </c>
     </row>
-    <row r="160" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="160" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B160">
         <v>0.54400902170848608</v>
       </c>
@@ -1692,7 +1688,7 @@
         <v>0.75717507753030733</v>
       </c>
     </row>
-    <row r="161" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B161">
         <v>0.54450202794051383</v>
       </c>
@@ -1700,7 +1696,7 @@
         <v>0.75175135196034248</v>
       </c>
     </row>
-    <row r="162" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B162">
         <v>0.54380053908355797</v>
       </c>
@@ -1708,7 +1704,7 @@
         <v>0.74311938454627124</v>
       </c>
     </row>
-    <row r="163" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B163">
         <v>0.54242593627724989</v>
       </c>
@@ -1716,7 +1712,7 @@
         <v>0.73383566238121845</v>
       </c>
     </row>
-    <row r="164" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B164">
         <v>0.53966312746678524</v>
       </c>
@@ -1724,7 +1720,7 @@
         <v>0.72653010172883425</v>
       </c>
     </row>
-    <row r="165" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B165">
         <v>0.53618784530386743</v>
       </c>
@@ -1732,7 +1728,7 @@
         <v>0.72212707182320435</v>
       </c>
     </row>
-    <row r="166" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B166">
         <v>0.53418850473464008</v>
       </c>
@@ -1740,7 +1736,7 @@
         <v>0.72283252587535796</v>
       </c>
     </row>
-    <row r="167" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B167">
         <v>0.53404149925697619</v>
       </c>
@@ -1748,7 +1744,7 @@
         <v>0.72924376685563319</v>
       </c>
     </row>
-    <row r="168" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B168">
         <v>0.53509013727327859</v>
       </c>
@@ -1756,7 +1752,7 @@
         <v>0.73975136446331125</v>
       </c>
     </row>
-    <row r="169" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="169" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B169">
         <v>0.5358777783906018</v>
       </c>
@@ -1764,7 +1760,7 @@
         <v>0.74873476366444225</v>
       </c>
     </row>
-    <row r="170" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B170">
         <v>0.5362358776522459</v>
       </c>
@@ -1772,7 +1768,7 @@
         <v>0.75270377514466802</v>
       </c>
     </row>
-    <row r="171" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B171">
         <v>0.53558669964275896</v>
       </c>
@@ -1780,7 +1776,7 @@
         <v>0.74918219291013999</v>
       </c>
     </row>
-    <row r="172" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B172">
         <v>0.53391684901531733</v>
       </c>
@@ -1788,7 +1784,7 @@
         <v>0.74091794310722114</v>
       </c>
     </row>
-    <row r="173" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B173">
         <v>0.53128227428385066</v>
       </c>
@@ -1796,7 +1792,7 @@
         <v>0.72996249388487255</v>
       </c>
     </row>
-    <row r="174" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="174" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B174">
         <v>0.527419789700728</v>
       </c>
@@ -1804,7 +1800,7 @@
         <v>0.71641520625505517</v>
       </c>
     </row>
-    <row r="175" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="175" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B175">
         <v>0.52270541724543229</v>
       </c>
@@ -1812,7 +1808,7 @@
         <v>0.70135911956405594</v>
       </c>
     </row>
-    <row r="176" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B176">
         <v>0.5299020403745196</v>
       </c>
@@ -1820,7 +1816,7 @@
         <v>0.70630134762136709</v>
       </c>
     </row>
-    <row r="177" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B177">
         <v>0.5462803009194761</v>
       </c>
@@ -1828,7 +1824,7 @@
         <v>0.72987183059348004</v>
       </c>
     </row>
-    <row r="178" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B178">
         <v>0.56164148351648358</v>
       </c>
@@ -1836,7 +1832,7 @@
         <v>0.75581444597069602</v>
       </c>
     </row>
-    <row r="179" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="179" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B179">
         <v>0.5654402026832499</v>
       </c>
@@ -1844,7 +1840,7 @@
         <v>0.76329648183336218</v>
       </c>
     </row>
-    <row r="180" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="180" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B180">
         <v>0.56006613832031471</v>
       </c>
@@ -1852,7 +1848,7 @@
         <v>0.75372655225497465</v>
       </c>
     </row>
-    <row r="181" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B181">
         <v>0.55475113122171948</v>
       </c>
@@ -1860,7 +1856,7 @@
         <v>0.7422087104072399</v>
       </c>
     </row>
-    <row r="182" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="182" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B182">
         <v>0.54943264801707681</v>
       </c>
@@ -1868,7 +1864,7 @@
         <v>0.73065947646331875</v>
       </c>
     </row>
-    <row r="183" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="183" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B183">
         <v>0.54621330943311663</v>
       </c>
@@ -1876,7 +1872,7 @@
         <v>0.72294924938382255</v>
       </c>
     </row>
-    <row r="184" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="184" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B184">
         <v>0.54571989896154927</v>
       </c>
@@ -1884,7 +1880,7 @@
         <v>0.72112096547852944</v>
       </c>
     </row>
-    <row r="185" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B185">
         <v>0.54711657826430415</v>
       </c>
@@ -1892,7 +1888,7 @@
         <v>0.72446958582552756</v>
       </c>
     </row>
-    <row r="186" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="186" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B186">
         <v>0.55039508839747597</v>
       </c>
@@ -1900,7 +1896,7 @@
         <v>0.73141038030811201</v>
       </c>
     </row>
-    <row r="187" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="187" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B187">
         <v>0.55484832845920062</v>
       </c>
@@ -1908,7 +1904,7 @@
         <v>0.74069556740638787</v>
       </c>
     </row>
-    <row r="188" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="188" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B188">
         <v>0.55630928427709114</v>
       </c>
@@ -1916,7 +1912,7 @@
         <v>0.74622880137970682</v>
       </c>
     </row>
-    <row r="189" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="189" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B189">
         <v>0.55428375207462943</v>
       </c>
@@ -1924,7 +1920,7 @@
         <v>0.74811079951925818</v>
       </c>
     </row>
-    <row r="190" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="190" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B190">
         <v>0.5502894766715859</v>
       </c>
@@ -1932,7 +1928,7 @@
         <v>0.74821092064933581</v>
       </c>
     </row>
-    <row r="191" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="191" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B191">
         <v>0.54707608941070218</v>
       </c>
@@ -1940,7 +1936,7 @@
         <v>0.75218898171144732</v>
       </c>
     </row>
-    <row r="192" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="192" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B192">
         <v>0.54409532909898262</v>
       </c>
@@ -1948,7 +1944,7 @@
         <v>0.75903827778090049</v>
       </c>
     </row>
-    <row r="193" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="193" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B193">
         <v>0.54122586062132649</v>
       </c>
@@ -1956,7 +1952,7 @@
         <v>0.76620095158130408</v>
       </c>
     </row>
-    <row r="194" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="194" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B194">
         <v>0.53869744619159132</v>
       </c>
@@ -1964,7 +1960,7 @@
         <v>0.77181052748968426</v>
       </c>
     </row>
-    <row r="195" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="195" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B195">
         <v>0.53722960573875334</v>
       </c>
@@ -1972,7 +1968,7 @@
         <v>0.77547350275259974</v>
       </c>
     </row>
-    <row r="196" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="196" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B196">
         <v>0.53816645354978587</v>
       </c>
@@ -1980,7 +1976,7 @@
         <v>0.77930394173569795</v>
       </c>
     </row>
-    <row r="197" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="197" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B197">
         <v>0.5411050462292526</v>
       </c>
@@ -1988,7 +1984,7 @@
         <v>0.78192102038542943</v>
       </c>
     </row>
-    <row r="198" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="198" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B198">
         <v>0.54296395491574601</v>
       </c>
@@ -1996,7 +1992,7 @@
         <v>0.78007421046758185</v>
       </c>
     </row>
-    <row r="199" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="199" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B199">
         <v>0.54386945344808313</v>
       </c>
@@ -2004,7 +2000,7 @@
         <v>0.77293785626466971</v>
       </c>
     </row>
-    <row r="200" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="200" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B200">
         <v>0.54481251050950052</v>
       </c>
@@ -2012,7 +2008,7 @@
         <v>0.76581189395213278</v>
       </c>
     </row>
-    <row r="201" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="201" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B201">
         <v>0.54641266978526737</v>
       </c>
@@ -2020,7 +2016,7 @@
         <v>0.76321817054613084</v>
       </c>
     </row>
-    <row r="202" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="202" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B202">
         <v>0.5484951731970471</v>
       </c>
@@ -2028,7 +2024,7 @@
         <v>0.76499943214082911</v>
       </c>
     </row>
-    <row r="203" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="203" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B203">
         <v>0.54555750608754749</v>
       </c>
@@ -2036,7 +2032,7 @@
         <v>0.75705249447873624</v>
       </c>
     </row>
-    <row r="204" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="204" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B204">
         <v>0.53968343062415802</v>
       </c>
@@ -2044,7 +2040,7 @@
         <v>0.74019196228109563</v>
       </c>
     </row>
-    <row r="205" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="205" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B205">
         <v>0.53391526743022355</v>
       </c>
@@ -2052,7 +2048,7 @@
         <v>0.72146280440342492</v>
       </c>
     </row>
-    <row r="206" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="206" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B206">
         <v>0.52917172162788129</v>
       </c>
@@ -2060,7 +2056,7 @@
         <v>0.70716885408624675</v>
       </c>
     </row>
-    <row r="207" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="207" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B207">
         <v>0.52613393297866506</v>
       </c>
@@ -2068,7 +2064,7 @@
         <v>0.7006767948225745</v>
       </c>
     </row>
-    <row r="208" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="208" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B208">
         <v>0.5306867190091783</v>
       </c>
@@ -2076,7 +2072,7 @@
         <v>0.70580670131593493</v>
       </c>
     </row>
-    <row r="209" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="209" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B209">
         <v>0.54054814564691323</v>
       </c>
@@ -2084,7 +2080,7 @@
         <v>0.7170808711801453</v>
       </c>
     </row>
-    <row r="210" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="210" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B210">
         <v>0.54719235364396657</v>
       </c>
@@ -2092,7 +2088,7 @@
         <v>0.72196620583717364</v>
       </c>
     </row>
-    <row r="211" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="211" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B211">
         <v>0.55013132351261851</v>
       </c>
@@ -2100,7 +2096,7 @@
         <v>0.72191618134064184</v>
       </c>
     </row>
-    <row r="212" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="212" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B212">
         <v>0.55048488305761545</v>
       </c>
@@ -2108,7 +2104,7 @@
         <v>0.7223958927552766</v>
       </c>
     </row>
-    <row r="213" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="213" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B213">
         <v>0.54948494678732007</v>
       </c>
@@ -2116,7 +2112,7 @@
         <v>0.7275613226338854</v>
       </c>
     </row>
-    <row r="214" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="214" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B214">
         <v>0.54767309875141879</v>
       </c>
@@ -2124,7 +2120,7 @@
         <v>0.73639103291713948</v>
       </c>
     </row>
-    <row r="215" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="215" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B215">
         <v>0.54777758807125387</v>
       </c>
@@ -2132,7 +2128,7 @@
         <v>0.74823629844630357</v>
       </c>
     </row>
-    <row r="216" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="216" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B216">
         <v>0.54894323844435544</v>
       </c>
@@ -2140,7 +2136,7 @@
         <v>0.75961910762357521</v>
       </c>
     </row>
-    <row r="217" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="217" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B217">
         <v>0.55053974484789014</v>
       </c>
@@ -2148,7 +2144,7 @@
         <v>0.77056745367430579</v>
       </c>
     </row>
-    <row r="218" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="218" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B218">
         <v>0.55205304175875314</v>
       </c>
@@ -2156,7 +2152,7 @@
         <v>0.78203675700825881</v>
       </c>
     </row>
-    <row r="219" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="219" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B219">
         <v>0.55319398091223138</v>
       </c>
@@ -2164,7 +2160,7 @@
         <v>0.79426254464547097</v>
       </c>
     </row>
-    <row r="220" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="220" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B220">
         <v>0.5524479624743478</v>
       </c>
@@ -2172,7 +2168,7 @@
         <v>0.80221577250073306</v>
       </c>
     </row>
-    <row r="221" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="221" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B221">
         <v>0.55012868507253154</v>
       </c>
@@ -2180,7 +2176,7 @@
         <v>0.80584990641085641</v>
       </c>
     </row>
-    <row r="222" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="222" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B222">
         <v>0.54820118756549074</v>
       </c>
@@ -2188,7 +2184,7 @@
         <v>0.80532541623006171</v>
       </c>
     </row>
-    <row r="223" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="223" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B223">
         <v>0.54773753037842832</v>
       </c>
@@ -2196,7 +2192,7 @@
         <v>0.80054681171160735</v>
       </c>
     </row>
-    <row r="224" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="224" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B224">
         <v>0.54788853777650104</v>
       </c>
@@ -2204,7 +2200,7 @@
         <v>0.79277104280379207</v>
       </c>
     </row>
-    <row r="225" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="225" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B225">
         <v>0.54520015989949167</v>
       </c>
@@ -2212,7 +2208,7 @@
         <v>0.7851584718177147</v>
       </c>
     </row>
-    <row r="226" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="226" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B226">
         <v>0.54058349415370643</v>
       </c>
@@ -2220,7 +2216,7 @@
         <v>0.77851458735384271</v>
       </c>
     </row>
-    <row r="227" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="227" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B227">
         <v>0.53468811741462041</v>
       </c>
@@ -2228,7 +2224,7 @@
         <v>0.77515664690939889</v>
       </c>
     </row>
-    <row r="228" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="228" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B228">
         <v>0.52789482555199729</v>
       </c>
@@ -2236,7 +2232,7 @@
         <v>0.77544693522107977</v>
       </c>
     </row>
-    <row r="229" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="229" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B229">
         <v>0.5222508687366888</v>
       </c>
@@ -2244,7 +2240,7 @@
         <v>0.77962392108508027</v>
       </c>
     </row>
-    <row r="230" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="230" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B230">
         <v>0.52455596278545258</v>
       </c>
@@ -2252,7 +2248,7 @@
         <v>0.78999097829151399</v>
       </c>
     </row>
-    <row r="231" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="231" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B231">
         <v>0.53300593878483327</v>
       </c>
@@ -2260,7 +2256,7 @@
         <v>0.80188042485153033</v>
       </c>
     </row>
-    <row r="232" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="232" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B232">
         <v>0.54032443626323057</v>
       </c>
@@ -2268,7 +2264,7 @@
         <v>0.80556776346065351</v>
       </c>
     </row>
-    <row r="233" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="233" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B233">
         <v>0.54625144175317186</v>
       </c>
@@ -2276,7 +2272,7 @@
         <v>0.80288869665513263</v>
       </c>
     </row>
-    <row r="234" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="234" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B234">
         <v>0.5499971216395142</v>
       </c>
@@ -2284,7 +2280,7 @@
         <v>0.79624719359852636</v>
       </c>
     </row>
-    <row r="235" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="235" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B235">
         <v>0.54996282102613969</v>
       </c>
@@ -2292,7 +2288,7 @@
         <v>0.78673053823714467</v>
       </c>
     </row>
-    <row r="236" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="236" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B236">
         <v>0.546875</v>
       </c>
@@ -2300,7 +2296,7 @@
         <v>0.77447860054347828</v>
       </c>
     </row>
-    <row r="237" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="237" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B237">
         <v>0.54506582648812874</v>
       </c>
@@ -2308,7 +2304,7 @@
         <v>0.76481996174187006</v>
       </c>
     </row>
-    <row r="238" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="238" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B238">
         <v>0.54429244225162599</v>
       </c>
@@ -2316,7 +2312,7 @@
         <v>0.75634166853554607</v>
       </c>
     </row>
-    <row r="239" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="239" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B239">
         <v>0.54299932900917014</v>
       </c>
@@ -2324,7 +2320,7 @@
         <v>0.74811787072243341</v>
       </c>
     </row>
-    <row r="240" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="240" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B240">
         <v>0.54021066711252308</v>
       </c>
@@ -2332,7 +2328,7 @@
         <v>0.73903973694476965</v>
       </c>
     </row>
-    <row r="241" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="241" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B241">
         <v>0.53642825410928474</v>
       </c>
@@ -2340,7 +2336,7 @@
         <v>0.7301338294091515</v>
       </c>
     </row>
-    <row r="242" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="242" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B242">
         <v>0.53473380015560745</v>
       </c>
@@ -2348,7 +2344,7 @@
         <v>0.72778259419806601</v>
       </c>
     </row>
-    <row r="243" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="243" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B243">
         <v>0.53396110770602323</v>
       </c>
@@ -2356,7 +2352,7 @@
         <v>0.73442190895414272</v>
       </c>
     </row>
-    <row r="244" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="244" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B244">
         <v>0.53385853167951725</v>
       </c>
@@ -2364,7 +2360,7 @@
         <v>0.74655659850262601</v>
       </c>
     </row>
-    <row r="245" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="245" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B245">
         <v>0.53435627485019888</v>
       </c>
@@ -2372,7 +2368,7 @@
         <v>0.75814526516212144</v>
       </c>
     </row>
-    <row r="246" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="246" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B246">
         <v>0.5356761915455005</v>
       </c>
@@ -2380,7 +2376,7 @@
         <v>0.76547409195531357</v>
       </c>
     </row>
-    <row r="247" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="247" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B247">
         <v>0.53824905575286097</v>
       </c>
@@ -2388,7 +2384,7 @@
         <v>0.77026495292857566</v>
       </c>
     </row>
-    <row r="248" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="248" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B248">
         <v>0.54195962803356779</v>
       </c>
@@ -2396,7 +2392,7 @@
         <v>0.77500567022000466</v>
       </c>
     </row>
-    <row r="249" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="249" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B249">
         <v>0.54018437871161129</v>
       </c>
@@ -2404,7 +2400,7 @@
         <v>0.77177704880945641</v>
       </c>
     </row>
-    <row r="250" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="250" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B250">
         <v>0.53275158024277003</v>
       </c>
@@ -2412,7 +2408,7 @@
         <v>0.76000559377971688</v>
       </c>
     </row>
-    <row r="251" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="251" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B251">
         <v>0.52384105960264904</v>
       </c>
@@ -2420,7 +2416,7 @@
         <v>0.74431070640176611</v>
       </c>
     </row>
-    <row r="252" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="252" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B252">
         <v>0.52059308072487631</v>
       </c>
@@ -2428,7 +2424,7 @@
         <v>0.73335475013728713</v>
       </c>
     </row>
-    <row r="253" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="253" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B253">
         <v>0.52281746031746035</v>
       </c>
@@ -2436,7 +2432,7 @@
         <v>0.72819058641975321</v>
       </c>
     </row>
-    <row r="254" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="254" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B254">
         <v>0.52853805073431237</v>
       </c>
@@ -2444,7 +2440,7 @@
         <v>0.7291967067200712</v>
       </c>
     </row>
-    <row r="255" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="255" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B255">
         <v>0.53711642599277976</v>
       </c>
@@ -2452,7 +2448,7 @@
         <v>0.73822314981949444</v>
       </c>
     </row>
-    <row r="256" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="256" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B256">
         <v>0.54394977168949776</v>
       </c>
@@ -2460,7 +2456,7 @@
         <v>0.74825913242009134</v>
       </c>
     </row>
-    <row r="257" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="257" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B257">
         <v>0.54355659783789967</v>
       </c>
@@ -2468,7 +2464,7 @@
         <v>0.75035806211748568</v>
       </c>
     </row>
-    <row r="258" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="258" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B258">
         <v>0.53728456856834073</v>
       </c>
@@ -2476,7 +2472,7 @@
         <v>0.74332119902167104</v>
       </c>
     </row>
-    <row r="259" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="259" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B259">
         <v>0.53126952570292529</v>
       </c>
@@ -2484,7 +2480,7 @@
         <v>0.73429650667424029</v>
       </c>
     </row>
-    <row r="260" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="260" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B260">
         <v>0.52530997611193264</v>
       </c>
@@ -2492,7 +2488,7 @@
         <v>0.72391878057103864</v>
       </c>
     </row>
-    <row r="261" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="261" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B261">
         <v>0.51970302684180469</v>
       </c>
@@ -2500,7 +2496,7 @@
         <v>0.71466876070816687</v>
       </c>
     </row>
-    <row r="262" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="262" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B262">
         <v>0.51440068985340615</v>
       </c>
@@ -2508,7 +2504,7 @@
         <v>0.70859902270767461</v>
       </c>
     </row>
-    <row r="263" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="263" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B263">
         <v>0.50912673118154961</v>
       </c>
@@ -2516,7 +2512,7 @@
         <v>0.70585327693110045</v>
       </c>
     </row>
-    <row r="264" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="264" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B264">
         <v>0.50565597667638484</v>
       </c>
@@ -2524,7 +2520,7 @@
         <v>0.70304489795918368</v>
       </c>
     </row>
-    <row r="265" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="265" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B265">
         <v>0.50290101388970276</v>
       </c>
@@ -2532,7 +2528,7 @@
         <v>0.70015999531149264</v>
       </c>
     </row>
-    <row r="266" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="266" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B266">
         <v>0.50052984811020851</v>
       </c>
@@ -2540,7 +2536,7 @@
         <v>0.69776462969504305</v>
       </c>
     </row>
-    <row r="267" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="267" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B267">
         <v>0.49840350047303694</v>
       </c>
@@ -2548,7 +2544,7 @@
         <v>0.69687559129612109</v>
       </c>
     </row>
-    <row r="268" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="268" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B268">
         <v>0.49776878681501757</v>
       </c>
@@ -2556,7 +2552,7 @@
         <v>0.6990242161004343</v>
       </c>
     </row>
-    <row r="269" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="269" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B269">
         <v>0.50399322362052268</v>
       </c>
@@ -2564,7 +2560,7 @@
         <v>0.71038661665053238</v>
       </c>
     </row>
-    <row r="270" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="270" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B270">
         <v>0.51619910625620646</v>
       </c>
@@ -2572,7 +2568,7 @@
         <v>0.73007075471698102</v>
       </c>
     </row>
-    <row r="271" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="271" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B271">
         <v>0.52840368137099336</v>
       </c>
@@ -2580,7 +2576,7 @@
         <v>0.75063598857505553</v>
       </c>
     </row>
-    <row r="272" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="272" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B272">
         <v>0.54010349288486426</v>
       </c>
@@ -2588,7 +2584,7 @@
         <v>0.77184993531694701</v>
       </c>
     </row>
-    <row r="273" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="273" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B273">
         <v>0.55030128373067855</v>
       </c>
@@ -2596,7 +2592,7 @@
         <v>0.7908704479958083</v>
       </c>
     </row>
-    <row r="274" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="274" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B274">
         <v>0.55701093719300554</v>
       </c>
@@ -2604,7 +2600,7 @@
         <v>0.80118016896980826</v>
       </c>
     </row>
-    <row r="275" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="275" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B275">
         <v>0.56110534509600418</v>
       </c>
@@ -2612,7 +2608,7 @@
         <v>0.8034723663726</v>
       </c>
     </row>
-    <row r="276" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="276" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B276">
         <v>0.55638426722764067</v>
       </c>
@@ -2620,7 +2616,7 @@
         <v>0.79828902913240263</v>
       </c>
     </row>
-    <row r="277" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="277" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B277">
         <v>0.54606083271004735</v>
       </c>
@@ -2628,7 +2624,7 @@
         <v>0.78721515831463484</v>
       </c>
     </row>
-    <row r="278" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="278" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B278">
         <v>0.53454700959130075</v>
       </c>
@@ -2636,7 +2632,7 @@
         <v>0.77568391471684295</v>
       </c>
     </row>
-    <row r="279" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="279" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B279">
         <v>0.52498792853693865</v>
       </c>
@@ -2644,7 +2640,7 @@
         <v>0.7676170931916948</v>
       </c>
     </row>
-    <row r="280" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="280" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B280">
         <v>0.51686067442697714</v>
       </c>
@@ -2652,7 +2648,7 @@
         <v>0.76248049921996897</v>
       </c>
     </row>
-    <row r="281" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="281" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B281">
         <v>0.51350378105869643</v>
       </c>
@@ -2660,7 +2656,7 @@
         <v>0.76033969511463229</v>
       </c>
     </row>
-    <row r="282" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="282" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B282">
         <v>0.51304767070451396</v>
       </c>
@@ -2668,7 +2664,7 @@
         <v>0.75942867474236131</v>
       </c>
     </row>
-    <row r="283" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="283" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B283">
         <v>0.51346118942464769</v>
       </c>
@@ -2676,7 +2672,7 @@
         <v>0.75693266380301294</v>
       </c>
     </row>
-    <row r="284" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="284" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B284">
         <v>0.5139410837677294</v>
       </c>
@@ -2684,7 +2680,7 @@
         <v>0.75307128136743839</v>
       </c>
     </row>
-    <row r="285" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="285" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B285">
         <v>0.51474335638878776</v>
       </c>
@@ -2692,7 +2688,7 @@
         <v>0.74931258342434159</v>
       </c>
     </row>
-    <row r="286" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="286" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B286">
         <v>0.51793557833089299</v>
       </c>
@@ -2700,7 +2696,7 @@
         <v>0.74988286969253282</v>
       </c>
     </row>
-    <row r="287" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="287" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B287">
         <v>0.52282795963573714</v>
       </c>
@@ -2708,7 +2704,7 @@
         <v>0.7550707605217819</v>
       </c>
     </row>
-    <row r="288" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="288" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B288">
         <v>0.52624087139497466</v>
       </c>
@@ -2716,7 +2712,7 @@
         <v>0.76226946404257945</v>
       </c>
     </row>
-    <row r="289" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="289" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B289">
         <v>0.52815196474020731</v>
       </c>
@@ -2724,7 +2720,7 @@
         <v>0.77200322800918741</v>
       </c>
     </row>
-    <row r="290" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="290" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B290">
         <v>0.52941542288557208</v>
       </c>
@@ -2732,7 +2728,7 @@
         <v>0.7828202736318407</v>
       </c>
     </row>
-    <row r="291" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="291" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B291">
         <v>0.53119151590767311</v>
       </c>
@@ -2740,7 +2736,7 @@
         <v>0.79019401122894561</v>
       </c>
     </row>
-    <row r="292" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="292" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B292">
         <v>0.53314969010204716</v>
       </c>
@@ -2748,7 +2744,7 @@
         <v>0.7886013898453641</v>
       </c>
     </row>
-    <row r="293" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="293" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B293">
         <v>0.53642592243384246</v>
       </c>
@@ -2756,7 +2752,7 @@
         <v>0.77789490225658442</v>
       </c>
     </row>
-    <row r="294" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="294" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B294">
         <v>0.54081697076835666</v>
       </c>
@@ -2764,7 +2760,7 @@
         <v>0.76358419092114416</v>
       </c>
     </row>
-    <row r="295" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="295" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B295">
         <v>0.54424610710216481</v>
       </c>
@@ -2772,7 +2768,7 @@
         <v>0.75285099379668308</v>
       </c>
     </row>
-    <row r="296" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="296" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B296">
         <v>0.54415666456096012</v>
       </c>
@@ -2780,7 +2776,7 @@
         <v>0.74769993682880598</v>
       </c>
     </row>
-    <row r="297" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="297" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B297">
         <v>0.54120603015075375</v>
       </c>
@@ -2788,7 +2784,7 @@
         <v>0.74768530150753765</v>
       </c>
     </row>
-    <row r="298" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="298" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B298">
         <v>0.54300296137609483</v>
       </c>
@@ -2796,7 +2792,7 @@
         <v>0.75752630584084191</v>
       </c>
     </row>
-    <row r="299" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="299" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B299">
         <v>0.54792169823312575</v>
       </c>
@@ -2804,7 +2800,7 @@
         <v>0.76745074361255872</v>
       </c>
     </row>
-    <row r="300" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="300" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B300">
         <v>0.5533350469091376</v>
       </c>
@@ -2812,7 +2808,7 @@
         <v>0.77259542475260246</v>
       </c>
     </row>
-    <row r="301" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="301" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B301">
         <v>0.55746118365490804</v>
       </c>
@@ -2820,7 +2816,7 @@
         <v>0.77526343142987075</v>
       </c>
     </row>
-    <row r="302" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="302" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B302">
         <v>0.55977690288713911</v>
       </c>
@@ -2828,7 +2824,7 @@
         <v>0.78122506561679783</v>
       </c>
     </row>
-    <row r="303" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="303" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B303">
         <v>0.55296902742158205</v>
       </c>
@@ -2836,7 +2832,7 @@
         <v>0.78940816729137897</v>
       </c>
     </row>
-    <row r="304" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="304" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B304">
         <v>0.54014024510125169</v>
       </c>
@@ -2844,7 +2840,7 @@
         <v>0.79804050068811849</v>
       </c>
     </row>
-    <row r="305" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="305" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B305">
         <v>0.52967378488143579</v>
       </c>
@@ -2852,7 +2848,7 @@
         <v>0.81166579326608146</v>
       </c>
     </row>
-    <row r="306" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="306" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B306">
         <v>0.52355883127138714</v>
       </c>
@@ -2860,7 +2856,7 @@
         <v>0.83197617794156364</v>
       </c>
     </row>
-    <row r="307" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="307" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B307">
         <v>0.52025416997617158</v>
       </c>
@@ -2868,7 +2864,7 @@
         <v>0.85728554408260504</v>
       </c>
     </row>
-    <row r="308" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="308" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B308">
         <v>0.51532252772491638</v>
       </c>
@@ -2876,7 +2872,7 @@
         <v>0.87065096134916986</v>
       </c>
     </row>
-    <row r="309" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="309" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B309">
         <v>0.50943396226415094</v>
       </c>
@@ -2884,7 +2880,7 @@
         <v>0.87025436280507418</v>
       </c>
     </row>
-    <row r="310" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="310" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B310">
         <v>0.51261688228512881</v>
       </c>
@@ -2892,7 +2888,7 @@
         <v>0.87352312027667478</v>
       </c>
     </row>
-    <row r="311" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="311" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B311">
         <v>0.52382794866834337</v>
       </c>
@@ -2900,7 +2896,7 @@
         <v>0.87975688398787655</v>
       </c>
     </row>
-    <row r="312" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="312" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B312">
         <v>0.53812479581836004</v>
       </c>
@@ -2908,7 +2904,7 @@
         <v>0.8890532505717087</v>
       </c>
     </row>
-    <row r="313" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="313" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B313">
         <v>0.54794158461640119</v>
       </c>
@@ -2916,7 +2912,7 @@
         <v>0.89734355382277142</v>
       </c>
     </row>
-    <row r="314" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="314" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B314">
         <v>0.55431661881551719</v>
       </c>
@@ -2924,7 +2920,7 @@
         <v>0.90671229218134464</v>
       </c>
     </row>
-    <row r="315" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="315" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B315">
         <v>0.55640203154236834</v>
       </c>
@@ -2932,7 +2928,7 @@
         <v>0.90934108527131785</v>
       </c>
     </row>
-    <row r="316" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="316" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B316">
         <v>0.55545218951425335</v>
       </c>
@@ -2940,7 +2936,7 @@
         <v>0.90698252375573141</v>
       </c>
     </row>
-    <row r="317" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="317" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B317">
         <v>0.5572145877378436</v>
       </c>
@@ -2948,7 +2944,7 @@
         <v>0.90568313953488389</v>
       </c>
     </row>
-    <row r="318" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="318" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B318">
         <v>0.56685163165543673</v>
       </c>
@@ -2956,7 +2952,7 @@
         <v>0.91103117981239279</v>
       </c>
     </row>
-    <row r="319" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="319" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B319">
         <v>0.58297928836962287</v>
       </c>
@@ -2964,7 +2960,7 @@
         <v>0.92219397238449263</v>
       </c>
     </row>
-    <row r="320" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="320" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B320">
         <v>0.58411519416210578</v>
       </c>
@@ -2972,7 +2968,7 @@
         <v>0.91104052645295797</v>
       </c>
     </row>
-    <row r="321" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="321" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B321">
         <v>0.57765977621847142</v>
       </c>
@@ -2980,7 +2976,7 @@
         <v>0.88765029395031281</v>
       </c>
     </row>
-    <row r="322" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="322" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B322">
         <v>0.56843524077931618</v>
       </c>
@@ -2988,7 +2984,7 @@
         <v>0.86162847690234035</v>
       </c>
     </row>
-    <row r="323" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="323" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B323">
         <v>0.55873242792470812</v>
       </c>
@@ -2996,7 +2992,7 @@
         <v>0.83712115796997866</v>
       </c>
     </row>
-    <row r="324" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="324" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B324">
         <v>0.54882721783557831</v>
       </c>
@@ -3004,7 +3000,7 @@
         <v>0.81434393869019972</v>
       </c>
     </row>
-    <row r="325" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="325" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B325">
         <v>0.54174259681093406</v>
       </c>
@@ -3012,7 +3008,7 @@
         <v>0.79627619589977228</v>
       </c>
     </row>
-    <row r="326" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="326" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B326">
         <v>0.53591438816674131</v>
       </c>
@@ -3020,7 +3016,7 @@
         <v>0.78011317794710888</v>
       </c>
     </row>
-    <row r="327" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="327" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B327">
         <v>0.53339636282742897</v>
       </c>
@@ -3028,7 +3024,7 @@
         <v>0.77061787442300211</v>
       </c>
     </row>
-    <row r="328" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="328" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B328">
         <v>0.53385634006565408</v>
       </c>
@@ -3036,7 +3032,7 @@
         <v>0.7676375674623046</v>
       </c>
     </row>
-    <row r="329" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="329" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B329">
         <v>0.535670356703567</v>
       </c>
@@ -3044,7 +3040,7 @@
         <v>0.76894554400089454</v>
       </c>
     </row>
-    <row r="330" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="330" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B330">
         <v>0.53654839434089374</v>
       </c>
@@ -3052,7 +3048,7 @@
         <v>0.77071524814731629</v>
       </c>
     </row>
-    <row r="331" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="331" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B331">
         <v>0.53686999661743151</v>
       </c>
@@ -3060,7 +3056,7 @@
         <v>0.77321795016349082</v>
       </c>
     </row>
-    <row r="332" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="332" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B332">
         <v>0.53554315350357973</v>
       </c>
@@ -3068,7 +3064,7 @@
         <v>0.77228141383392546</v>
       </c>
     </row>
-    <row r="333" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="333" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B333">
         <v>0.53292504775817517</v>
       </c>
@@ -3076,7 +3072,7 @@
         <v>0.76768738060456243</v>
       </c>
     </row>
-    <row r="334" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="334" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B334">
         <v>0.53064082455747252</v>
       </c>
@@ -3084,7 +3080,7 @@
         <v>0.7614138471879901</v>
       </c>
     </row>
-    <row r="335" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="335" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B335">
         <v>0.53066606812187878</v>
       </c>
@@ -3092,7 +3088,7 @@
         <v>0.75702990853487484</v>
       </c>
     </row>
-    <row r="336" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="336" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B336">
         <v>0.5322316846201568</v>
       </c>
@@ -3100,7 +3096,7 @@
         <v>0.75543567762675556</v>
       </c>
     </row>
-    <row r="337" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="337" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B337">
         <v>0.53467879476975555</v>
       </c>
@@ -3108,7 +3104,7 @@
         <v>0.75786355884025014</v>
       </c>
     </row>
-    <row r="338" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="338" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B338">
         <v>0.53778135048231512</v>
       </c>
@@ -3116,7 +3112,7 @@
         <v>0.76400206706476814</v>
       </c>
     </row>
-    <row r="339" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="339" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B339">
         <v>0.53925883034163291</v>
       </c>
@@ -3124,7 +3120,7 @@
         <v>0.77088071800810665</v>
       </c>
     </row>
-    <row r="340" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="340" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B340">
         <v>0.53753998255306779</v>
       </c>
@@ -3132,7 +3128,7 @@
         <v>0.77574934574004062</v>
       </c>
     </row>
-    <row r="341" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="341" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B341">
         <v>0.5336051252184042</v>
       </c>
@@ -3140,7 +3136,7 @@
         <v>0.77915958066394864</v>
       </c>
     </row>
-    <row r="342" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="342" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B342">
         <v>0.52674754477180818</v>
       </c>
@@ -3148,7 +3144,7 @@
         <v>0.77501386481802426</v>
       </c>
     </row>
-    <row r="343" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="343" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B343">
         <v>0.51855864074348601</v>
       </c>
@@ -3156,7 +3152,7 @@
         <v>0.76361024003649025</v>
       </c>
     </row>
-    <row r="344" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="344" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B344">
         <v>0.51224593209841784</v>
       </c>
@@ -3164,7 +3160,7 @@
         <v>0.74628568211249358</v>
       </c>
     </row>
-    <row r="345" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="345" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B345">
         <v>0.50858225590726702</v>
       </c>
@@ -3172,7 +3168,7 @@
         <v>0.72388709317877842</v>
       </c>
     </row>
-    <row r="346" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="346" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B346">
         <v>0.50685916583692892</v>
       </c>
@@ -3180,7 +3176,7 @@
         <v>0.70080097355902216</v>
       </c>
     </row>
-    <row r="347" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="347" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B347">
         <v>0.50680987709002323</v>
       </c>
@@ -3188,7 +3184,7 @@
         <v>0.68847193001882401</v>
       </c>
     </row>
-    <row r="348" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="348" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B348">
         <v>0.5085975882090219</v>
       </c>
@@ -3196,7 +3192,7 @@
         <v>0.68823246985261277</v>
       </c>
     </row>
-    <row r="349" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="349" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B349">
         <v>0.51377082624957493</v>
       </c>
@@ -3204,7 +3200,7 @@
         <v>0.69786920548566245</v>
       </c>
     </row>
-    <row r="350" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="350" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B350">
         <v>0.52237078196446141</v>
       </c>
@@ -3212,7 +3208,7 @@
         <v>0.71498003125542631</v>
       </c>
     </row>
-    <row r="351" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="351" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B351">
         <v>0.53167099976364929</v>
       </c>
@@ -3220,7 +3216,7 @@
         <v>0.73499054597021973</v>
       </c>
     </row>
-    <row r="352" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="352" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B352">
         <v>0.53512838801711848</v>
       </c>
@@ -3228,7 +3224,7 @@
         <v>0.74765275796481223</v>
       </c>
     </row>
-    <row r="353" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="353" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B353">
         <v>0.53271634048573446</v>
       </c>
@@ -3236,7 +3232,7 @@
         <v>0.75156979485970288</v>
       </c>
     </row>
-    <row r="354" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="354" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B354">
         <v>0.53066369606003749</v>
       </c>
@@ -3244,7 +3240,7 @@
         <v>0.75585952157598502</v>
       </c>
     </row>
-    <row r="355" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="355" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B355">
         <v>0.52874839312843291</v>
       </c>
@@ -3252,7 +3248,7 @@
         <v>0.75521327568072927</v>
       </c>
     </row>
-    <row r="356" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="356" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B356">
         <v>0.52776154295733491</v>
       </c>
@@ -3260,7 +3256,7 @@
         <v>0.75084161309175923</v>
       </c>
     </row>
-    <row r="357" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="357" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B357">
         <v>0.52855799741450227</v>
       </c>
@@ -3268,7 +3264,7 @@
         <v>0.74608649665060522</v>
       </c>
     </row>
-    <row r="358" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="358" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B358">
         <v>0.53034973325429768</v>
       </c>
@@ -3276,7 +3272,7 @@
         <v>0.74284825133372867</v>
       </c>
     </row>
-    <row r="359" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="359" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B359">
         <v>0.53526598924088464</v>
       </c>
@@ -3284,7 +3280,7 @@
         <v>0.74163538553496711</v>
       </c>
     </row>
-    <row r="360" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="360" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B360">
         <v>0.54211858279103387</v>
       </c>
@@ -3292,7 +3288,7 @@
         <v>0.74340503735839958</v>
       </c>
     </row>
-    <row r="361" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="361" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B361">
         <v>0.54503199323916451</v>
       </c>
@@ -3300,7 +3296,7 @@
         <v>0.74330435832427866</v>
       </c>
     </row>
-    <row r="362" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="362" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B362">
         <v>0.5414593201031237</v>
       </c>
@@ -3308,7 +3304,7 @@
         <v>0.7382840697883567</v>
       </c>
     </row>
-    <row r="363" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="363" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B363">
         <v>0.53370054489457475</v>
       </c>
@@ -3316,7 +3312,7 @@
         <v>0.72890547263681582</v>
       </c>
     </row>
-    <row r="364" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="364" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B364">
         <v>0.52960254747022051</v>
       </c>
@@ -3324,7 +3320,7 @@
         <v>0.72401757282698409</v>
       </c>
     </row>
-    <row r="365" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="365" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B365">
         <v>0.52748289690964845</v>
       </c>
@@ -3332,7 +3328,7 @@
         <v>0.72176456711488557</v>
       </c>
     </row>
-    <row r="366" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="366" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B366">
         <v>0.52705659707847885</v>
       </c>
@@ -3340,7 +3336,7 @@
         <v>0.72221479685374645</v>
       </c>
     </row>
-    <row r="367" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="367" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B367">
         <v>0.52780087917310214</v>
       </c>
@@ -3348,7 +3344,7 @@
         <v>0.72625341570630864</v>
       </c>
     </row>
-    <row r="368" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="368" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B368">
         <v>0.52924308501105199</v>
       </c>
@@ -3356,7 +3352,7 @@
         <v>0.73361192424876043</v>
       </c>
     </row>
-    <row r="369" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="369" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B369">
         <v>0.53055822906641004</v>
       </c>
@@ -3364,7 +3360,7 @@
         <v>0.74404054379210793</v>
       </c>
     </row>
-    <row r="370" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="370" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B370">
         <v>0.53176912816781863</v>
       </c>
@@ -3372,7 +3368,7 @@
         <v>0.75627682793743189</v>
       </c>
     </row>
-    <row r="371" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="371" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B371">
         <v>0.53133215137250112</v>
       </c>
@@ -3380,7 +3376,7 @@
         <v>0.767375435593324</v>
       </c>
     </row>
-    <row r="372" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="372" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B372">
         <v>0.52934286771051664</v>
       </c>
@@ -3388,7 +3384,7 @@
         <v>0.77505054863765266</v>
       </c>
     </row>
-    <row r="373" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="373" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B373">
         <v>0.52771908017402114</v>
       </c>
@@ -3396,7 +3392,7 @@
         <v>0.77870913610938475</v>
       </c>
     </row>
-    <row r="374" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="374" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B374">
         <v>0.52913898984835195</v>
       </c>
@@ -3404,7 +3400,7 @@
         <v>0.77877992229602699</v>
       </c>
     </row>
-    <row r="375" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="375" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B375">
         <v>0.53340919147860166</v>
       </c>
@@ -3412,7 +3408,7 @@
         <v>0.77575320816739346</v>
       </c>
     </row>
-    <row r="376" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="376" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B376">
         <v>0.53498282661239027</v>
       </c>
@@ -3420,7 +3416,7 @@
         <v>0.7696584404019845</v>
       </c>
     </row>
-    <row r="377" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="377" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B377">
         <v>0.53484954960710396</v>
       </c>
@@ -3428,7 +3424,7 @@
         <v>0.7639468472497285</v>
       </c>
     </row>
-    <row r="378" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="378" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B378">
         <v>0.53424833247819392</v>
       </c>
@@ -3436,7 +3432,7 @@
         <v>0.7614045664443303</v>
       </c>
     </row>
-    <row r="379" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="379" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B379">
         <v>0.53394306324874408</v>
       </c>
@@ -3444,7 +3440,7 @@
         <v>0.76283782043024606</v>
       </c>
     </row>
-    <row r="380" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="380" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B380">
         <v>0.53382923673997418</v>
       </c>
@@ -3452,7 +3448,7 @@
         <v>0.766173997412678</v>
       </c>
     </row>
-    <row r="381" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="381" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B381">
         <v>0.53508030431107345</v>
       </c>
@@ -3460,7 +3456,7 @@
         <v>0.77164575069900521</v>
       </c>
     </row>
-    <row r="382" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="382" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B382">
         <v>0.53704793669478779</v>
       </c>
@@ -3468,7 +3464,7 @@
         <v>0.77852331436792888</v>
       </c>
     </row>
-    <row r="383" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="383" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B383">
         <v>0.53690616411464465</v>
       </c>
@@ -3476,7 +3472,7 @@
         <v>0.78140753828032972</v>
       </c>
     </row>
-    <row r="384" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="384" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B384">
         <v>0.53399258343634115</v>
       </c>
@@ -3484,7 +3480,7 @@
         <v>0.77781471602368091</v>
       </c>
     </row>
-    <row r="385" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="385" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B385">
         <v>0.53051491912096416</v>
       </c>
@@ -3492,7 +3488,7 @@
         <v>0.76923503254495074</v>
       </c>
     </row>
-    <row r="386" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="386" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B386">
         <v>0.53673875377013414</v>
       </c>
@@ -3500,144 +3496,135 @@
         <v>0.76355323108515694</v>
       </c>
     </row>
-    <row r="387" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="387" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B387">
+        <v>0.54940052574212994</v>
+      </c>
+      <c r="C387">
+        <v>0.76302814643841776</v>
+      </c>
+    </row>
+    <row r="388" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B388">
         <v>0.55606494746895896</v>
       </c>
-      <c r="C387">
+      <c r="C388">
         <v>0.76295065265838902</v>
       </c>
     </row>
-    <row r="388" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B388">
+    <row r="389" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B389">
         <v>0.55614906051655877</v>
       </c>
-      <c r="C388">
+      <c r="C389">
         <v>0.76228680952680206</v>
       </c>
     </row>
-    <row r="389" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B389">
+    <row r="390" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B390">
         <v>0.55082230740694949</v>
       </c>
-      <c r="C389">
+      <c r="C390">
         <v>0.76002967725979975</v>
       </c>
     </row>
-    <row r="390" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B390">
+    <row r="391" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B391">
         <v>0.54030487804878047</v>
       </c>
-      <c r="C390">
+      <c r="C391">
         <v>0.75653963414634151</v>
       </c>
     </row>
-    <row r="391" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B391">
+    <row r="392" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B392">
         <v>0.52522880539499028</v>
       </c>
-      <c r="C391">
+      <c r="C392">
         <v>0.74991570327552992</v>
       </c>
     </row>
-    <row r="392" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B392">
+    <row r="393" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B393">
         <v>0.51625307937270926</v>
       </c>
-      <c r="C392">
+      <c r="C393">
         <v>0.74679324640990208</v>
       </c>
     </row>
-    <row r="393" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B393">
+    <row r="394" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B394">
         <v>0.51181911613566289</v>
       </c>
-      <c r="C393">
+      <c r="C394">
         <v>0.74586240251496283</v>
       </c>
     </row>
-    <row r="394" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B394">
+    <row r="395" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B395">
         <v>0.5125926833752068</v>
       </c>
-      <c r="C394">
+      <c r="C395">
         <v>0.74856179912984877</v>
       </c>
     </row>
-    <row r="395" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B395">
+    <row r="396" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B396">
         <v>0.51953491279614927</v>
       </c>
-      <c r="C395">
+      <c r="C396">
         <v>0.75464712133525047</v>
       </c>
     </row>
-    <row r="396" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B396">
+    <row r="397" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B397">
         <v>0.53157827312323858</v>
       </c>
-      <c r="C396">
+      <c r="C397">
         <v>0.76423264155777615</v>
       </c>
     </row>
-    <row r="397" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B397">
+    <row r="398" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B398">
         <v>0.54005953921822425</v>
       </c>
-      <c r="C397">
+      <c r="C398">
         <v>0.7655203209940461</v>
       </c>
     </row>
-    <row r="398" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B398">
+    <row r="399" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B399">
         <v>0.54563106796116501</v>
       </c>
-      <c r="C398">
+      <c r="C399">
         <v>0.76445242718446604</v>
       </c>
     </row>
-    <row r="399" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B399">
+    <row r="400" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B400">
         <v>0.548478414720453</v>
       </c>
-      <c r="C399">
+      <c r="C400">
         <v>0.76413562375345823</v>
       </c>
     </row>
-    <row r="400" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B400">
+    <row r="401" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B401">
         <v>0.54872219743802175</v>
       </c>
-      <c r="C400">
+      <c r="C401">
         <v>0.76476260276591679</v>
       </c>
     </row>
-    <row r="401" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B401">
+    <row r="402" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B402">
         <v>0.54667338075155802</v>
       </c>
-      <c r="C401">
+      <c r="C402">
         <v>0.76315541008371646</v>
-      </c>
-    </row>
-    <row r="402" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B402">
-        <v>8</v>
-      </c>
-      <c r="C402">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="403" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B403">
-        <v>5</v>
-      </c>
-      <c r="C403" s="2">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>